<commit_message>
Working with STATA file
</commit_message>
<xml_diff>
--- a/3_Toyota_Data_Modeling/STATA/1_STATA_Mode_Estimation Results.xlsx
+++ b/3_Toyota_Data_Modeling/STATA/1_STATA_Mode_Estimation Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ghasak/Desktop/Toyota_Project_Data_Wrangling/3_Toyota_Data_Modeling/STATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A30AAA4-ECC7-0543-BC8D-86B2339EE416}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0AD0345-E8E4-B640-8D95-9757BBCE0062}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="81">
   <si>
     <t>Upper</t>
   </si>
@@ -459,6 +459,10 @@
   </si>
   <si>
     <t>Major_prefectural_road</t>
+  </si>
+  <si>
+    <t>Road width collected from Police Report- Usui sensei dataset</t>
+    <phoneticPr fontId="13"/>
   </si>
 </sst>
 </file>
@@ -10323,7 +10327,7 @@
   <dimension ref="C2:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -10579,7 +10583,10 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="3:12" ht="16" thickBot="1">
+    <row r="15" spans="3:12" ht="17" thickBot="1">
+      <c r="C15" s="178" t="s">
+        <v>80</v>
+      </c>
       <c r="I15" s="190"/>
       <c r="J15" s="191"/>
       <c r="K15" s="192"/>

</xml_diff>

<commit_message>
Peparing the dummies for Toyota City variables
</commit_message>
<xml_diff>
--- a/3_Toyota_Data_Modeling/STATA/1_STATA_Mode_Estimation Results.xlsx
+++ b/3_Toyota_Data_Modeling/STATA/1_STATA_Mode_Estimation Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ghasak/Desktop/Toyota_Project_Data_Wrangling/3_Toyota_Data_Modeling/STATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BED88B3-A7AF-954F-8C41-58E85A213DF7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91673500-253E-844B-87D1-FDA7C8D58BAB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,8 @@
     <sheet name="Test " sheetId="1" r:id="rId1"/>
     <sheet name="Descriptive Statistic" sheetId="7" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="38" r:id="rId3"/>
-    <sheet name="Univaraite-All-Models" sheetId="28" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="39" r:id="rId4"/>
+    <sheet name="Univaraite-All-Models" sheetId="28" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="384">
   <si>
     <t>Upper</t>
   </si>
@@ -1352,14 +1353,125 @@
     <t>Arm4_2ndSide_Sidewalk_with_guardrail</t>
   </si>
   <si>
-    <t>Arm4_2ndSide_Sidewalk_without_any_guardrail_or_curbstone</t>
-  </si>
-  <si>
     <t>Road type is not existed (three arms only)</t>
     <phoneticPr fontId="13"/>
   </si>
   <si>
     <t>Arm4_Road_type_Non_Existed</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>Arm4_2ndSide_Sidewalk_without_any_guardrail_or_curbstone</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>Non_Existed (No fourth arm)</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>Variables of fifth and sixth--etc arm</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>Arm5_6_RoadType_Divided_roadway_with_No_Physical_Median_and_No_Central_Strip</t>
+  </si>
+  <si>
+    <t>Arm5_6_RoadType_Divided_roadway_with_No_Physical_Median_and_with_Central_Strip</t>
+  </si>
+  <si>
+    <t>Arm5_6_RoadType_Divided_roadway_with_Physical_Median_and_No_Central_Strip</t>
+  </si>
+  <si>
+    <t>Arm5_6_RoadType_Divided_roadway_with_Physical_Median_and_with_Central_Strip</t>
+  </si>
+  <si>
+    <t>Arm5_6_RoadType_One_way_street</t>
+  </si>
+  <si>
+    <t>Arm5_6_RoadType_Single_roadway_without_central_strip</t>
+  </si>
+  <si>
+    <t>Arm5_6_Road_type_Non_Existed</t>
+  </si>
+  <si>
+    <t>Arm5_6_Number_of_lanes_for_first_arm</t>
+  </si>
+  <si>
+    <t>Arm5_6_No_of_lanes_changed_at_the_approach</t>
+  </si>
+  <si>
+    <t>Arm5_6_Red/Yellow_flashing_signal</t>
+  </si>
+  <si>
+    <t>Arm5_6_Stop_sign</t>
+  </si>
+  <si>
+    <t>Arm5_6_Traffic_signal_with_left_or_right_turn_only</t>
+  </si>
+  <si>
+    <t>Arm5_6_Traffic_signal_without_left_or_right_turn_only</t>
+  </si>
+  <si>
+    <t>Arm5_6_Uncontroled</t>
+  </si>
+  <si>
+    <t>Arm5_6_Presence_of_pedestrian_traffic_signal</t>
+  </si>
+  <si>
+    <t>Arm5_6_Crossing_path_without_bicycle_only_path</t>
+  </si>
+  <si>
+    <t>Arm5_6_Crosswalk_existed_within_50m</t>
+  </si>
+  <si>
+    <t>Arm5_6_Crosswalk_path_with_bicycle_only_path</t>
+  </si>
+  <si>
+    <t>Arm5_6_1stSide_No_sidewalk</t>
+  </si>
+  <si>
+    <t>Arm5_6_1stSide_Sidewalk_with_curbstone</t>
+  </si>
+  <si>
+    <t>Arm5_6_1stSide_Sidewalk_with_guardrail</t>
+  </si>
+  <si>
+    <t>Arm5_6_1stSide_Sidewalk_without_any_guardrail_or_curbstone</t>
+  </si>
+  <si>
+    <t>Arm5_6_2ndSide_No_sidewalk</t>
+  </si>
+  <si>
+    <t>Arm5_6_2ndSide_Sidewalk_with_curbstone</t>
+  </si>
+  <si>
+    <t>Arm5_6_2ndSide_Sidewalk_with_guardrail</t>
+  </si>
+  <si>
+    <t>Arm5_6_2ndSide_Sidewalk_without_any_guardrail_or_curbstone</t>
+  </si>
+  <si>
+    <t>Arm5_6_Corsswalk_not_existed</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>mean arm. 1</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>mean arm 2]</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t xml:space="preserve">arm 3 </t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>arm 4</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> Traffic signal without left or right turn only </t>
     <phoneticPr fontId="13"/>
   </si>
 </sst>
@@ -1371,7 +1483,7 @@
     <numFmt numFmtId="176" formatCode="0.000"/>
     <numFmt numFmtId="177" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1556,8 +1668,13 @@
       <color rgb="FF000000"/>
       <name val="SF Pro Display Regular"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="SF Pro Display Regular"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1639,6 +1756,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF580"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9BFF8D"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3289,7 +3412,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="211">
+  <cellXfs count="220">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -3765,14 +3888,23 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1408">
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -10019,6 +10151,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF9BFF8D"/>
       <color rgb="FFFFF580"/>
       <color rgb="FFFF978A"/>
       <color rgb="FF009999"/>
@@ -11264,10 +11397,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89ABEEF7-365E-A345-AB58-564271AAE464}">
-  <dimension ref="C2:L242"/>
+  <dimension ref="C2:L286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
+    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D172" sqref="D172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -12677,7 +12810,7 @@
       <c r="H78" s="180"/>
       <c r="I78" s="180"/>
     </row>
-    <row r="79" spans="3:9">
+    <row r="79" spans="3:9" ht="16" thickBot="1">
       <c r="C79" s="180"/>
       <c r="D79" s="169"/>
       <c r="E79" s="169"/>
@@ -12686,16 +12819,16 @@
       <c r="H79" s="180"/>
       <c r="I79" s="180"/>
     </row>
-    <row r="80" spans="3:9" ht="16">
-      <c r="C80" s="203" t="s">
+    <row r="80" spans="3:9" ht="17" thickBot="1">
+      <c r="C80" s="214" t="s">
         <v>199</v>
       </c>
-      <c r="D80" s="204"/>
-      <c r="E80" s="204"/>
-      <c r="F80" s="204"/>
-      <c r="G80" s="204"/>
-      <c r="H80" s="204"/>
-      <c r="I80" s="204"/>
+      <c r="D80" s="215"/>
+      <c r="E80" s="215"/>
+      <c r="F80" s="215"/>
+      <c r="G80" s="215"/>
+      <c r="H80" s="215"/>
+      <c r="I80" s="216"/>
     </row>
     <row r="81" spans="3:9" ht="17" thickBot="1">
       <c r="C81" s="176" t="s">
@@ -13394,16 +13527,17 @@
         <v>238</v>
       </c>
     </row>
-    <row r="121" spans="3:9" ht="16">
-      <c r="C121" s="205" t="s">
+    <row r="120" spans="3:9" ht="16" thickBot="1"/>
+    <row r="121" spans="3:9" ht="17" thickBot="1">
+      <c r="C121" s="211" t="s">
         <v>263</v>
       </c>
-      <c r="D121" s="206"/>
-      <c r="E121" s="206"/>
-      <c r="F121" s="206"/>
-      <c r="G121" s="206"/>
-      <c r="H121" s="206"/>
-      <c r="I121" s="206"/>
+      <c r="D121" s="212"/>
+      <c r="E121" s="212"/>
+      <c r="F121" s="212"/>
+      <c r="G121" s="212"/>
+      <c r="H121" s="212"/>
+      <c r="I121" s="213"/>
     </row>
     <row r="122" spans="3:9" ht="17" thickBot="1">
       <c r="C122" s="176" t="s">
@@ -13865,6 +13999,7 @@
       <c r="C147" s="176" t="s">
         <v>223</v>
       </c>
+      <c r="D147" s="203"/>
     </row>
     <row r="148" spans="3:9">
       <c r="C148" s="195" t="s">
@@ -14102,16 +14237,17 @@
         <v>294</v>
       </c>
     </row>
-    <row r="162" spans="3:9" ht="16">
-      <c r="C162" s="207" t="s">
+    <row r="161" spans="3:9" ht="16" thickBot="1"/>
+    <row r="162" spans="3:9" ht="17" thickBot="1">
+      <c r="C162" s="208" t="s">
         <v>296</v>
       </c>
-      <c r="D162" s="208"/>
-      <c r="E162" s="208"/>
-      <c r="F162" s="208"/>
-      <c r="G162" s="208"/>
-      <c r="H162" s="208"/>
-      <c r="I162" s="208"/>
+      <c r="D162" s="209"/>
+      <c r="E162" s="209"/>
+      <c r="F162" s="209"/>
+      <c r="G162" s="209"/>
+      <c r="H162" s="209"/>
+      <c r="I162" s="210"/>
     </row>
     <row r="163" spans="3:9" ht="17" thickBot="1">
       <c r="C163" s="176" t="s">
@@ -14810,16 +14946,17 @@
         <v>321</v>
       </c>
     </row>
-    <row r="203" spans="3:9" ht="16">
-      <c r="C203" s="209" t="s">
+    <row r="202" spans="3:9" ht="16" thickBot="1"/>
+    <row r="203" spans="3:9" ht="17" thickBot="1">
+      <c r="C203" s="205" t="s">
         <v>322</v>
       </c>
-      <c r="D203" s="210"/>
-      <c r="E203" s="210"/>
-      <c r="F203" s="210"/>
-      <c r="G203" s="210"/>
-      <c r="H203" s="210"/>
-      <c r="I203" s="210"/>
+      <c r="D203" s="206"/>
+      <c r="E203" s="206"/>
+      <c r="F203" s="206"/>
+      <c r="G203" s="206"/>
+      <c r="H203" s="206"/>
+      <c r="I203" s="207"/>
     </row>
     <row r="204" spans="3:9" ht="17" thickBot="1">
       <c r="C204" s="176" t="s">
@@ -14953,8 +15090,8 @@
       </c>
     </row>
     <row r="211" spans="3:9" ht="16" thickBot="1">
-      <c r="C211" s="198" t="s">
-        <v>348</v>
+      <c r="C211" s="204" t="s">
+        <v>347</v>
       </c>
       <c r="D211" s="173">
         <v>9.8173499999999997E-2</v>
@@ -14970,22 +15107,31 @@
       </c>
       <c r="H211" s="182"/>
       <c r="I211" s="183" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="212" spans="3:9" ht="17" thickBot="1">
       <c r="C212" s="176" t="s">
         <v>207</v>
       </c>
+      <c r="D212" s="203"/>
     </row>
     <row r="213" spans="3:9">
       <c r="C213" s="195" t="s">
         <v>216</v>
       </c>
-      <c r="D213" s="165"/>
-      <c r="E213" s="165"/>
-      <c r="F213" s="165"/>
-      <c r="G213" s="165"/>
+      <c r="D213" s="165">
+        <v>1.8333330000000001</v>
+      </c>
+      <c r="E213" s="165">
+        <v>1.6114809999999999</v>
+      </c>
+      <c r="F213" s="165">
+        <v>0</v>
+      </c>
+      <c r="G213" s="165">
+        <v>6</v>
+      </c>
       <c r="H213" s="177"/>
       <c r="I213" s="178" t="s">
         <v>329</v>
@@ -14995,10 +15141,18 @@
       <c r="C214" s="179" t="s">
         <v>206</v>
       </c>
-      <c r="D214" s="169"/>
-      <c r="E214" s="169"/>
-      <c r="F214" s="169"/>
-      <c r="G214" s="169"/>
+      <c r="D214" s="169">
+        <v>0.30821920000000003</v>
+      </c>
+      <c r="E214" s="169">
+        <v>0.46228570000000002</v>
+      </c>
+      <c r="F214" s="169">
+        <v>0</v>
+      </c>
+      <c r="G214" s="169">
+        <v>1</v>
+      </c>
       <c r="H214" s="180"/>
       <c r="I214" s="181" t="s">
         <v>330</v>
@@ -15008,10 +15162,18 @@
       <c r="C215" s="179" t="s">
         <v>219</v>
       </c>
-      <c r="D215" s="169"/>
-      <c r="E215" s="169"/>
-      <c r="F215" s="169"/>
-      <c r="G215" s="169"/>
+      <c r="D215" s="169">
+        <v>2.7397299999999999E-2</v>
+      </c>
+      <c r="E215" s="169">
+        <v>0.16342470000000001</v>
+      </c>
+      <c r="F215" s="169">
+        <v>0</v>
+      </c>
+      <c r="G215" s="169">
+        <v>1</v>
+      </c>
       <c r="H215" s="180"/>
       <c r="I215" s="181" t="s">
         <v>272</v>
@@ -15021,10 +15183,18 @@
       <c r="C216" s="179" t="s">
         <v>220</v>
       </c>
-      <c r="D216" s="169"/>
-      <c r="E216" s="169"/>
-      <c r="F216" s="169"/>
-      <c r="G216" s="169"/>
+      <c r="D216" s="169">
+        <v>0.2899543</v>
+      </c>
+      <c r="E216" s="169">
+        <v>0.45425979999999999</v>
+      </c>
+      <c r="F216" s="169">
+        <v>0</v>
+      </c>
+      <c r="G216" s="169">
+        <v>1</v>
+      </c>
       <c r="H216" s="180"/>
       <c r="I216" s="181" t="s">
         <v>273</v>
@@ -15034,10 +15204,18 @@
       <c r="C217" s="179" t="s">
         <v>221</v>
       </c>
-      <c r="D217" s="169"/>
-      <c r="E217" s="169"/>
-      <c r="F217" s="169"/>
-      <c r="G217" s="169"/>
+      <c r="D217" s="169">
+        <v>0.35301369999999999</v>
+      </c>
+      <c r="E217" s="169">
+        <v>1.973786</v>
+      </c>
+      <c r="F217" s="169">
+        <v>0</v>
+      </c>
+      <c r="G217" s="169">
+        <v>30</v>
+      </c>
       <c r="H217" s="180"/>
       <c r="I217" s="181" t="s">
         <v>274</v>
@@ -15047,10 +15225,18 @@
       <c r="C218" s="179" t="s">
         <v>222</v>
       </c>
-      <c r="D218" s="169"/>
-      <c r="E218" s="169"/>
-      <c r="F218" s="169"/>
-      <c r="G218" s="169"/>
+      <c r="D218" s="169">
+        <v>0.10045659999999999</v>
+      </c>
+      <c r="E218" s="169">
+        <v>0.30095159999999999</v>
+      </c>
+      <c r="F218" s="169">
+        <v>0</v>
+      </c>
+      <c r="G218" s="169">
+        <v>1</v>
+      </c>
       <c r="H218" s="180"/>
       <c r="I218" s="181" t="s">
         <v>275</v>
@@ -15060,10 +15246,18 @@
       <c r="C219" s="179" t="s">
         <v>217</v>
       </c>
-      <c r="D219" s="169"/>
-      <c r="E219" s="169"/>
-      <c r="F219" s="169"/>
-      <c r="G219" s="169"/>
+      <c r="D219" s="169">
+        <v>0.59344750000000002</v>
+      </c>
+      <c r="E219" s="169">
+        <v>1.393475</v>
+      </c>
+      <c r="F219" s="169">
+        <v>0</v>
+      </c>
+      <c r="G219" s="169">
+        <v>15.5</v>
+      </c>
       <c r="H219" s="180"/>
       <c r="I219" s="181" t="s">
         <v>276</v>
@@ -15073,10 +15267,18 @@
       <c r="C220" s="179" t="s">
         <v>218</v>
       </c>
-      <c r="D220" s="169"/>
-      <c r="E220" s="169"/>
-      <c r="F220" s="169"/>
-      <c r="G220" s="169"/>
+      <c r="D220" s="169">
+        <v>0.23287669999999999</v>
+      </c>
+      <c r="E220" s="169">
+        <v>0.42314770000000002</v>
+      </c>
+      <c r="F220" s="169">
+        <v>0</v>
+      </c>
+      <c r="G220" s="169">
+        <v>1</v>
+      </c>
       <c r="H220" s="180"/>
       <c r="I220" s="181" t="s">
         <v>277</v>
@@ -15086,10 +15288,18 @@
       <c r="C221" s="198" t="s">
         <v>227</v>
       </c>
-      <c r="D221" s="173"/>
-      <c r="E221" s="173"/>
-      <c r="F221" s="173"/>
-      <c r="G221" s="173"/>
+      <c r="D221" s="173">
+        <v>0.1780822</v>
+      </c>
+      <c r="E221" s="173">
+        <v>0.38301940000000001</v>
+      </c>
+      <c r="F221" s="173">
+        <v>0</v>
+      </c>
+      <c r="G221" s="173">
+        <v>1</v>
+      </c>
       <c r="H221" s="182"/>
       <c r="I221" s="183" t="s">
         <v>225</v>
@@ -15104,10 +15314,18 @@
       <c r="C223" s="195" t="s">
         <v>250</v>
       </c>
-      <c r="D223" s="165"/>
-      <c r="E223" s="165"/>
-      <c r="F223" s="165"/>
-      <c r="G223" s="165"/>
+      <c r="D223" s="165">
+        <v>4.5662000000000003E-3</v>
+      </c>
+      <c r="E223" s="165">
+        <v>6.7496399999999998E-2</v>
+      </c>
+      <c r="F223" s="165">
+        <v>0</v>
+      </c>
+      <c r="G223" s="165">
+        <v>1</v>
+      </c>
       <c r="H223" s="177"/>
       <c r="I223" s="178" t="s">
         <v>331</v>
@@ -15117,10 +15335,18 @@
       <c r="C224" s="179" t="s">
         <v>245</v>
       </c>
-      <c r="D224" s="169"/>
-      <c r="E224" s="169"/>
-      <c r="F224" s="169"/>
-      <c r="G224" s="169"/>
+      <c r="D224" s="169">
+        <v>4.3379000000000001E-2</v>
+      </c>
+      <c r="E224" s="169">
+        <v>0.2039417</v>
+      </c>
+      <c r="F224" s="169">
+        <v>0</v>
+      </c>
+      <c r="G224" s="169">
+        <v>1</v>
+      </c>
       <c r="H224" s="180"/>
       <c r="I224" s="181" t="s">
         <v>332</v>
@@ -15130,10 +15356,18 @@
       <c r="C225" s="179" t="s">
         <v>246</v>
       </c>
-      <c r="D225" s="169"/>
-      <c r="E225" s="169"/>
-      <c r="F225" s="169"/>
-      <c r="G225" s="169"/>
+      <c r="D225" s="169">
+        <v>0.15068490000000001</v>
+      </c>
+      <c r="E225" s="169">
+        <v>0.35815059999999999</v>
+      </c>
+      <c r="F225" s="169">
+        <v>0</v>
+      </c>
+      <c r="G225" s="169">
+        <v>1</v>
+      </c>
       <c r="H225" s="180"/>
       <c r="I225" s="181" t="s">
         <v>333</v>
@@ -15143,10 +15377,18 @@
       <c r="C226" s="179" t="s">
         <v>247</v>
       </c>
-      <c r="D226" s="169"/>
-      <c r="E226" s="169"/>
-      <c r="F226" s="169"/>
-      <c r="G226" s="169"/>
+      <c r="D226" s="169">
+        <v>0.39497719999999997</v>
+      </c>
+      <c r="E226" s="169">
+        <v>0.48940479999999997</v>
+      </c>
+      <c r="F226" s="169">
+        <v>0</v>
+      </c>
+      <c r="G226" s="169">
+        <v>1</v>
+      </c>
       <c r="H226" s="180"/>
       <c r="I226" s="181" t="s">
         <v>334</v>
@@ -15156,10 +15398,18 @@
       <c r="C227" s="179" t="s">
         <v>248</v>
       </c>
-      <c r="D227" s="169"/>
-      <c r="E227" s="169"/>
-      <c r="F227" s="169"/>
-      <c r="G227" s="169"/>
+      <c r="D227" s="169">
+        <v>5.7077599999999999E-2</v>
+      </c>
+      <c r="E227" s="169">
+        <v>0.2322562</v>
+      </c>
+      <c r="F227" s="169">
+        <v>0</v>
+      </c>
+      <c r="G227" s="169">
+        <v>1</v>
+      </c>
       <c r="H227" s="180"/>
       <c r="I227" s="181" t="s">
         <v>335</v>
@@ -15169,10 +15419,18 @@
       <c r="C228" s="198" t="s">
         <v>249</v>
       </c>
-      <c r="D228" s="173"/>
-      <c r="E228" s="173"/>
-      <c r="F228" s="173"/>
-      <c r="G228" s="173"/>
+      <c r="D228" s="173">
+        <v>0.37214609999999998</v>
+      </c>
+      <c r="E228" s="173">
+        <v>0.48392980000000002</v>
+      </c>
+      <c r="F228" s="173">
+        <v>0</v>
+      </c>
+      <c r="G228" s="173">
+        <v>1</v>
+      </c>
       <c r="H228" s="182"/>
       <c r="I228" s="183" t="s">
         <v>336</v>
@@ -15182,15 +15440,24 @@
       <c r="C230" s="176" t="s">
         <v>223</v>
       </c>
+      <c r="D230" s="203"/>
     </row>
     <row r="231" spans="3:9">
       <c r="C231" s="195" t="s">
         <v>251</v>
       </c>
-      <c r="D231" s="165"/>
-      <c r="E231" s="165"/>
-      <c r="F231" s="165"/>
-      <c r="G231" s="165"/>
+      <c r="D231" s="165">
+        <v>0.31278539999999999</v>
+      </c>
+      <c r="E231" s="165">
+        <v>0.46415790000000001</v>
+      </c>
+      <c r="F231" s="165">
+        <v>0</v>
+      </c>
+      <c r="G231" s="165">
+        <v>1</v>
+      </c>
       <c r="H231" s="177"/>
       <c r="I231" s="178" t="s">
         <v>337</v>
@@ -15200,135 +15467,792 @@
       <c r="C232" s="179" t="s">
         <v>252</v>
       </c>
-      <c r="D232" s="169"/>
-      <c r="E232" s="169"/>
-      <c r="F232" s="169"/>
-      <c r="G232" s="169"/>
+      <c r="D232" s="169">
+        <v>0.1027397</v>
+      </c>
+      <c r="E232" s="169">
+        <v>0.30396580000000001</v>
+      </c>
+      <c r="F232" s="169">
+        <v>0</v>
+      </c>
+      <c r="G232" s="169">
+        <v>1</v>
+      </c>
       <c r="H232" s="180"/>
       <c r="I232" s="181" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="233" spans="3:9" ht="16" thickBot="1">
-      <c r="C233" s="198" t="s">
+    <row r="233" spans="3:9">
+      <c r="C233" s="179" t="s">
         <v>253</v>
       </c>
-      <c r="D233" s="173"/>
-      <c r="E233" s="173"/>
-      <c r="F233" s="173"/>
-      <c r="G233" s="173"/>
-      <c r="H233" s="182"/>
-      <c r="I233" s="183" t="s">
+      <c r="D233" s="169">
+        <v>0.2351598</v>
+      </c>
+      <c r="E233" s="169">
+        <v>0.42458360000000001</v>
+      </c>
+      <c r="F233" s="169">
+        <v>0</v>
+      </c>
+      <c r="G233" s="169">
+        <v>1</v>
+      </c>
+      <c r="H233" s="180"/>
+      <c r="I233" s="181" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="234" spans="3:9" ht="17" thickBot="1">
-      <c r="C234" s="176" t="s">
+    <row r="234" spans="3:9" ht="16" thickBot="1">
+      <c r="C234" s="204" t="s">
+        <v>350</v>
+      </c>
+      <c r="D234" s="173">
+        <v>0.34931509999999999</v>
+      </c>
+      <c r="E234" s="173">
+        <v>0.47729880000000002</v>
+      </c>
+      <c r="F234" s="173">
+        <v>0</v>
+      </c>
+      <c r="G234" s="173">
+        <v>1</v>
+      </c>
+      <c r="H234" s="182"/>
+      <c r="I234" s="183"/>
+    </row>
+    <row r="235" spans="3:9" ht="17" thickBot="1">
+      <c r="C235" s="176" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="235" spans="3:9">
-      <c r="C235" s="195" t="s">
+    <row r="236" spans="3:9">
+      <c r="C236" s="195" t="s">
         <v>254</v>
       </c>
-      <c r="D235" s="165"/>
-      <c r="E235" s="165"/>
-      <c r="F235" s="165"/>
-      <c r="G235" s="165"/>
-      <c r="H235" s="177"/>
-      <c r="I235" s="178" t="s">
+      <c r="D236" s="165">
+        <v>0.54337899999999995</v>
+      </c>
+      <c r="E236" s="165">
+        <v>0.49868430000000002</v>
+      </c>
+      <c r="F236" s="165">
+        <v>0</v>
+      </c>
+      <c r="G236" s="165">
+        <v>1</v>
+      </c>
+      <c r="H236" s="177"/>
+      <c r="I236" s="178" t="s">
         <v>340</v>
-      </c>
-    </row>
-    <row r="236" spans="3:9">
-      <c r="C236" s="179" t="s">
-        <v>255</v>
-      </c>
-      <c r="D236" s="169"/>
-      <c r="E236" s="169"/>
-      <c r="F236" s="169"/>
-      <c r="G236" s="169"/>
-      <c r="H236" s="180"/>
-      <c r="I236" s="181" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="237" spans="3:9">
       <c r="C237" s="179" t="s">
-        <v>256</v>
-      </c>
-      <c r="D237" s="169"/>
-      <c r="E237" s="169"/>
-      <c r="F237" s="169"/>
-      <c r="G237" s="169"/>
+        <v>255</v>
+      </c>
+      <c r="D237" s="169">
+        <v>0.1552511</v>
+      </c>
+      <c r="E237" s="169">
+        <v>0.36255799999999999</v>
+      </c>
+      <c r="F237" s="169">
+        <v>0</v>
+      </c>
+      <c r="G237" s="169">
+        <v>1</v>
+      </c>
       <c r="H237" s="180"/>
       <c r="I237" s="181" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="238" spans="3:9">
       <c r="C238" s="179" t="s">
-        <v>257</v>
-      </c>
-      <c r="D238" s="169"/>
-      <c r="E238" s="169"/>
-      <c r="F238" s="169"/>
-      <c r="G238" s="169"/>
+        <v>256</v>
+      </c>
+      <c r="D238" s="169">
+        <v>0.26255709999999999</v>
+      </c>
+      <c r="E238" s="169">
+        <v>0.4405269</v>
+      </c>
+      <c r="F238" s="169">
+        <v>0</v>
+      </c>
+      <c r="G238" s="169">
+        <v>1</v>
+      </c>
       <c r="H238" s="180"/>
       <c r="I238" s="181" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="239" spans="3:9">
       <c r="C239" s="179" t="s">
-        <v>258</v>
-      </c>
-      <c r="D239" s="169"/>
-      <c r="E239" s="169"/>
-      <c r="F239" s="169"/>
-      <c r="G239" s="169"/>
+        <v>257</v>
+      </c>
+      <c r="D239" s="169">
+        <v>3.8812800000000001E-2</v>
+      </c>
+      <c r="E239" s="169">
+        <v>0.1933694</v>
+      </c>
+      <c r="F239" s="169">
+        <v>0</v>
+      </c>
+      <c r="G239" s="169">
+        <v>1</v>
+      </c>
       <c r="H239" s="180"/>
       <c r="I239" s="181" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="240" spans="3:9">
       <c r="C240" s="179" t="s">
-        <v>259</v>
-      </c>
-      <c r="D240" s="169"/>
-      <c r="E240" s="169"/>
-      <c r="F240" s="169"/>
-      <c r="G240" s="169"/>
+        <v>258</v>
+      </c>
+      <c r="D240" s="169">
+        <v>0.14383560000000001</v>
+      </c>
+      <c r="E240" s="169">
+        <v>0.35132429999999998</v>
+      </c>
+      <c r="F240" s="169">
+        <v>0</v>
+      </c>
+      <c r="G240" s="169">
+        <v>1</v>
+      </c>
       <c r="H240" s="180"/>
       <c r="I240" s="181" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="241" spans="3:9">
       <c r="C241" s="179" t="s">
-        <v>260</v>
-      </c>
-      <c r="D241" s="169"/>
-      <c r="E241" s="169"/>
-      <c r="F241" s="169"/>
-      <c r="G241" s="169"/>
+        <v>259</v>
+      </c>
+      <c r="D241" s="169">
+        <v>0.173516</v>
+      </c>
+      <c r="E241" s="169">
+        <v>0.37912580000000001</v>
+      </c>
+      <c r="F241" s="169">
+        <v>0</v>
+      </c>
+      <c r="G241" s="169">
+        <v>1</v>
+      </c>
       <c r="H241" s="180"/>
       <c r="I241" s="181" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="242" spans="3:9">
+      <c r="C242" s="179" t="s">
+        <v>260</v>
+      </c>
+      <c r="D242" s="169">
+        <v>0.30821920000000003</v>
+      </c>
+      <c r="E242" s="169">
+        <v>0.46228570000000002</v>
+      </c>
+      <c r="F242" s="169">
+        <v>0</v>
+      </c>
+      <c r="G242" s="169">
+        <v>1</v>
+      </c>
+      <c r="H242" s="180"/>
+      <c r="I242" s="181" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="242" spans="3:9" ht="16" thickBot="1">
-      <c r="C242" s="198" t="s">
+    <row r="243" spans="3:9" ht="16" thickBot="1">
+      <c r="C243" s="198" t="s">
         <v>261</v>
       </c>
-      <c r="D242" s="173"/>
-      <c r="E242" s="173"/>
-      <c r="F242" s="173"/>
-      <c r="G242" s="173"/>
-      <c r="H242" s="182"/>
-      <c r="I242" s="183" t="s">
+      <c r="D243" s="173">
+        <v>2.51142E-2</v>
+      </c>
+      <c r="E243" s="173">
+        <v>0.15665080000000001</v>
+      </c>
+      <c r="F243" s="173">
+        <v>0</v>
+      </c>
+      <c r="G243" s="173">
+        <v>1</v>
+      </c>
+      <c r="H243" s="182"/>
+      <c r="I243" s="183" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="244" spans="3:9">
+      <c r="D244" s="203"/>
+    </row>
+    <row r="245" spans="3:9" ht="16" thickBot="1">
+      <c r="D245" s="203"/>
+    </row>
+    <row r="246" spans="3:9" ht="17" thickBot="1">
+      <c r="C246" s="217" t="s">
+        <v>351</v>
+      </c>
+      <c r="D246" s="218"/>
+      <c r="E246" s="218"/>
+      <c r="F246" s="218"/>
+      <c r="G246" s="218"/>
+      <c r="H246" s="218"/>
+      <c r="I246" s="219"/>
+    </row>
+    <row r="247" spans="3:9" ht="17" thickBot="1">
+      <c r="C247" s="176" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="248" spans="3:9">
+      <c r="C248" s="195" t="s">
+        <v>200</v>
+      </c>
+      <c r="D248" s="165">
+        <v>2.2831000000000001E-3</v>
+      </c>
+      <c r="E248" s="165">
+        <v>4.7781799999999999E-2</v>
+      </c>
+      <c r="F248" s="165">
+        <v>0</v>
+      </c>
+      <c r="G248" s="165">
+        <v>1</v>
+      </c>
+      <c r="H248" s="177"/>
+      <c r="I248" s="178" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="249" spans="3:9">
+      <c r="C249" s="179" t="s">
+        <v>205</v>
+      </c>
+      <c r="H249" s="180"/>
+      <c r="I249" s="181" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="250" spans="3:9">
+      <c r="C250" s="179" t="s">
+        <v>203</v>
+      </c>
+      <c r="D250" s="169"/>
+      <c r="E250" s="169"/>
+      <c r="F250" s="169"/>
+      <c r="G250" s="169"/>
+      <c r="H250" s="180"/>
+      <c r="I250" s="181" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="251" spans="3:9">
+      <c r="C251" s="179" t="s">
+        <v>204</v>
+      </c>
+      <c r="D251" s="169"/>
+      <c r="E251" s="169"/>
+      <c r="F251" s="169"/>
+      <c r="G251" s="169"/>
+      <c r="H251" s="180"/>
+      <c r="I251" s="181" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="252" spans="3:9">
+      <c r="C252" s="179" t="s">
+        <v>201</v>
+      </c>
+      <c r="D252" s="169"/>
+      <c r="E252" s="169"/>
+      <c r="F252" s="169"/>
+      <c r="G252" s="169"/>
+      <c r="H252" s="180"/>
+      <c r="I252" s="181" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="253" spans="3:9">
+      <c r="C253" s="179" t="s">
+        <v>202</v>
+      </c>
+      <c r="D253" s="169"/>
+      <c r="E253" s="169"/>
+      <c r="F253" s="169"/>
+      <c r="G253" s="169"/>
+      <c r="H253" s="180"/>
+      <c r="I253" s="181" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="254" spans="3:9" ht="16" thickBot="1">
+      <c r="C254" s="204" t="s">
         <v>347</v>
+      </c>
+      <c r="D254" s="169">
+        <v>0.99771690000000002</v>
+      </c>
+      <c r="E254" s="169">
+        <v>4.7781799999999999E-2</v>
+      </c>
+      <c r="F254" s="169">
+        <v>0</v>
+      </c>
+      <c r="G254" s="169">
+        <v>1</v>
+      </c>
+      <c r="H254" s="182"/>
+      <c r="I254" s="183" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="255" spans="3:9" ht="17" thickBot="1">
+      <c r="C255" s="176" t="s">
+        <v>207</v>
+      </c>
+      <c r="D255" s="203"/>
+    </row>
+    <row r="256" spans="3:9">
+      <c r="C256" s="195" t="s">
+        <v>216</v>
+      </c>
+      <c r="D256" s="165">
+        <v>9.1324000000000006E-3</v>
+      </c>
+      <c r="E256" s="165">
+        <v>0.1911274</v>
+      </c>
+      <c r="F256" s="165">
+        <v>0</v>
+      </c>
+      <c r="G256" s="165">
+        <v>4</v>
+      </c>
+      <c r="H256" s="177"/>
+      <c r="I256" s="178" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="257" spans="3:9">
+      <c r="C257" s="179" t="s">
+        <v>206</v>
+      </c>
+      <c r="D257" s="169"/>
+      <c r="E257" s="169"/>
+      <c r="F257" s="169"/>
+      <c r="G257" s="169"/>
+      <c r="H257" s="180"/>
+      <c r="I257" s="181" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="258" spans="3:9">
+      <c r="C258" s="179" t="s">
+        <v>219</v>
+      </c>
+      <c r="D258" s="169"/>
+      <c r="E258" s="169"/>
+      <c r="F258" s="169"/>
+      <c r="G258" s="169"/>
+      <c r="H258" s="180"/>
+      <c r="I258" s="181" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="259" spans="3:9">
+      <c r="C259" s="179" t="s">
+        <v>220</v>
+      </c>
+      <c r="D259" s="169"/>
+      <c r="E259" s="169"/>
+      <c r="F259" s="169"/>
+      <c r="G259" s="169"/>
+      <c r="H259" s="180"/>
+      <c r="I259" s="181" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="260" spans="3:9">
+      <c r="C260" s="179" t="s">
+        <v>221</v>
+      </c>
+      <c r="D260" s="169"/>
+      <c r="E260" s="169"/>
+      <c r="F260" s="169"/>
+      <c r="G260" s="169"/>
+      <c r="H260" s="180"/>
+      <c r="I260" s="181" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="261" spans="3:9">
+      <c r="C261" s="179" t="s">
+        <v>222</v>
+      </c>
+      <c r="D261" s="169"/>
+      <c r="E261" s="169"/>
+      <c r="F261" s="169"/>
+      <c r="G261" s="169"/>
+      <c r="H261" s="180"/>
+      <c r="I261" s="181" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="262" spans="3:9">
+      <c r="C262" s="179" t="s">
+        <v>217</v>
+      </c>
+      <c r="D262" s="169">
+        <v>1.0821900000000001E-2</v>
+      </c>
+      <c r="E262" s="169">
+        <v>0.22648599999999999</v>
+      </c>
+      <c r="F262" s="169">
+        <v>0</v>
+      </c>
+      <c r="G262" s="169">
+        <v>4.74</v>
+      </c>
+      <c r="H262" s="180"/>
+      <c r="I262" s="181" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="263" spans="3:9">
+      <c r="C263" s="179" t="s">
+        <v>218</v>
+      </c>
+      <c r="D263" s="169">
+        <v>2.2831000000000001E-3</v>
+      </c>
+      <c r="E263" s="169">
+        <v>4.7781799999999999E-2</v>
+      </c>
+      <c r="F263" s="169">
+        <v>0</v>
+      </c>
+      <c r="G263" s="169">
+        <v>1</v>
+      </c>
+      <c r="H263" s="180"/>
+      <c r="I263" s="181" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="264" spans="3:9" ht="16" thickBot="1">
+      <c r="C264" s="198" t="s">
+        <v>227</v>
+      </c>
+      <c r="D264" s="173"/>
+      <c r="E264" s="173"/>
+      <c r="F264" s="173"/>
+      <c r="G264" s="173"/>
+      <c r="H264" s="182"/>
+      <c r="I264" s="183" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="265" spans="3:9" ht="17" thickBot="1">
+      <c r="C265" s="176" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="266" spans="3:9">
+      <c r="C266" s="195" t="s">
+        <v>250</v>
+      </c>
+      <c r="D266" s="165"/>
+      <c r="E266" s="165"/>
+      <c r="F266" s="165"/>
+      <c r="G266" s="165"/>
+      <c r="H266" s="177"/>
+      <c r="I266" s="178" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="267" spans="3:9">
+      <c r="C267" s="179" t="s">
+        <v>245</v>
+      </c>
+      <c r="D267" s="169"/>
+      <c r="E267" s="169"/>
+      <c r="F267" s="169"/>
+      <c r="G267" s="169"/>
+      <c r="H267" s="180"/>
+      <c r="I267" s="181" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="268" spans="3:9">
+      <c r="C268" s="179" t="s">
+        <v>246</v>
+      </c>
+      <c r="D268" s="169"/>
+      <c r="E268" s="169"/>
+      <c r="F268" s="169"/>
+      <c r="G268" s="169"/>
+      <c r="H268" s="180"/>
+      <c r="I268" s="181" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="269" spans="3:9">
+      <c r="C269" s="179" t="s">
+        <v>247</v>
+      </c>
+      <c r="D269" s="169"/>
+      <c r="E269" s="169"/>
+      <c r="F269" s="169"/>
+      <c r="G269" s="169"/>
+      <c r="H269" s="180"/>
+      <c r="I269" s="181" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="270" spans="3:9">
+      <c r="C270" s="179" t="s">
+        <v>248</v>
+      </c>
+      <c r="D270" s="180">
+        <v>2.2831000000000001E-3</v>
+      </c>
+      <c r="E270" s="180">
+        <v>4.7781799999999999E-2</v>
+      </c>
+      <c r="F270" s="180">
+        <v>0</v>
+      </c>
+      <c r="G270" s="180">
+        <v>1</v>
+      </c>
+      <c r="H270" s="180"/>
+      <c r="I270" s="181" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="271" spans="3:9" ht="16" thickBot="1">
+      <c r="C271" s="198" t="s">
+        <v>249</v>
+      </c>
+      <c r="D271" s="182"/>
+      <c r="E271" s="182"/>
+      <c r="F271" s="182"/>
+      <c r="G271" s="182"/>
+      <c r="H271" s="182"/>
+      <c r="I271" s="183" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="273" spans="3:9" ht="17" thickBot="1">
+      <c r="C273" s="176" t="s">
+        <v>223</v>
+      </c>
+      <c r="D273" s="203"/>
+    </row>
+    <row r="274" spans="3:9">
+      <c r="C274" s="195" t="s">
+        <v>251</v>
+      </c>
+      <c r="D274" s="177"/>
+      <c r="E274" s="177"/>
+      <c r="F274" s="177"/>
+      <c r="G274" s="177"/>
+      <c r="H274" s="177"/>
+      <c r="I274" s="178" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="275" spans="3:9">
+      <c r="C275" s="179" t="s">
+        <v>252</v>
+      </c>
+      <c r="D275" s="169"/>
+      <c r="E275" s="169"/>
+      <c r="F275" s="169"/>
+      <c r="G275" s="169"/>
+      <c r="H275" s="180"/>
+      <c r="I275" s="181" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="276" spans="3:9">
+      <c r="C276" s="179" t="s">
+        <v>253</v>
+      </c>
+      <c r="D276" s="180">
+        <v>2.2831000000000001E-3</v>
+      </c>
+      <c r="E276" s="180">
+        <v>4.7781799999999999E-2</v>
+      </c>
+      <c r="F276" s="180">
+        <v>0</v>
+      </c>
+      <c r="G276" s="180">
+        <v>1</v>
+      </c>
+      <c r="H276" s="180"/>
+      <c r="I276" s="181" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="277" spans="3:9" ht="16" thickBot="1">
+      <c r="C277" s="204" t="s">
+        <v>350</v>
+      </c>
+      <c r="D277" s="173"/>
+      <c r="E277" s="173"/>
+      <c r="F277" s="173"/>
+      <c r="G277" s="173"/>
+      <c r="H277" s="182"/>
+      <c r="I277" s="183" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="278" spans="3:9" ht="17" thickBot="1">
+      <c r="C278" s="176" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="279" spans="3:9">
+      <c r="C279" s="195" t="s">
+        <v>254</v>
+      </c>
+      <c r="D279" s="165">
+        <v>0.99771690000000002</v>
+      </c>
+      <c r="E279" s="165">
+        <v>4.7781799999999999E-2</v>
+      </c>
+      <c r="F279" s="165">
+        <v>0</v>
+      </c>
+      <c r="G279" s="165">
+        <v>1</v>
+      </c>
+      <c r="H279" s="177"/>
+      <c r="I279" s="178" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="280" spans="3:9">
+      <c r="C280" s="179" t="s">
+        <v>255</v>
+      </c>
+      <c r="D280" s="169">
+        <v>2.2831000000000001E-3</v>
+      </c>
+      <c r="E280" s="169">
+        <v>4.7781799999999999E-2</v>
+      </c>
+      <c r="F280" s="169">
+        <v>0</v>
+      </c>
+      <c r="G280" s="169">
+        <v>1</v>
+      </c>
+      <c r="H280" s="180"/>
+      <c r="I280" s="181" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="281" spans="3:9">
+      <c r="C281" s="179" t="s">
+        <v>256</v>
+      </c>
+      <c r="H281" s="180"/>
+      <c r="I281" s="181" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="282" spans="3:9">
+      <c r="C282" s="179" t="s">
+        <v>257</v>
+      </c>
+      <c r="D282" s="169"/>
+      <c r="E282" s="169"/>
+      <c r="F282" s="169"/>
+      <c r="G282" s="169"/>
+      <c r="H282" s="180"/>
+      <c r="I282" s="181" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="283" spans="3:9">
+      <c r="C283" s="179" t="s">
+        <v>258</v>
+      </c>
+      <c r="D283" s="169">
+        <v>2.2831000000000001E-3</v>
+      </c>
+      <c r="E283" s="169">
+        <v>4.7781799999999999E-2</v>
+      </c>
+      <c r="F283" s="169">
+        <v>0</v>
+      </c>
+      <c r="G283" s="169">
+        <v>1</v>
+      </c>
+      <c r="H283" s="180"/>
+      <c r="I283" s="181" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="284" spans="3:9">
+      <c r="C284" s="179" t="s">
+        <v>259</v>
+      </c>
+      <c r="D284" s="169"/>
+      <c r="E284" s="169"/>
+      <c r="F284" s="169"/>
+      <c r="G284" s="169"/>
+      <c r="H284" s="180"/>
+      <c r="I284" s="181" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="285" spans="3:9">
+      <c r="C285" s="179" t="s">
+        <v>260</v>
+      </c>
+      <c r="D285" s="169"/>
+      <c r="E285" s="169"/>
+      <c r="F285" s="169"/>
+      <c r="G285" s="169"/>
+      <c r="H285" s="180"/>
+      <c r="I285" s="181" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="286" spans="3:9" ht="16" thickBot="1">
+      <c r="C286" s="198" t="s">
+        <v>261</v>
+      </c>
+      <c r="D286" s="173"/>
+      <c r="E286" s="173"/>
+      <c r="F286" s="173"/>
+      <c r="G286" s="173"/>
+      <c r="H286" s="182"/>
+      <c r="I286" s="183" t="s">
+        <v>377</v>
       </c>
     </row>
   </sheetData>
@@ -15348,6 +16272,422 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A347DF6-38A4-3E4F-B1CD-97279C107F51}">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" zoomScale="193" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="1" width="53.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="19" thickBot="1">
+      <c r="A1" s="214" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" s="215"/>
+    </row>
+    <row r="2" spans="1:6" ht="19" thickBot="1">
+      <c r="A2" s="176" t="s">
+        <v>295</v>
+      </c>
+      <c r="B2" s="160" t="s">
+        <v>379</v>
+      </c>
+      <c r="C2" s="160" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2" t="s">
+        <v>381</v>
+      </c>
+      <c r="E2" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="195" t="s">
+        <v>200</v>
+      </c>
+      <c r="B3" s="165">
+        <v>0.43379000000000001</v>
+      </c>
+      <c r="C3" s="165">
+        <v>0.44748860000000001</v>
+      </c>
+      <c r="D3" s="165">
+        <v>0.43835619999999997</v>
+      </c>
+      <c r="E3" s="165">
+        <v>0.2420091</v>
+      </c>
+      <c r="F3" s="165">
+        <v>2.2831000000000001E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="179" t="s">
+        <v>205</v>
+      </c>
+      <c r="B4" s="169">
+        <v>0.26255709999999999</v>
+      </c>
+      <c r="C4" s="169">
+        <v>0.23972599999999999</v>
+      </c>
+      <c r="D4" s="169">
+        <v>0.24885840000000001</v>
+      </c>
+      <c r="E4" s="169">
+        <v>0.1917808</v>
+      </c>
+      <c r="F4" s="160"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="179" t="s">
+        <v>203</v>
+      </c>
+      <c r="B5" s="169">
+        <v>0.13698630000000001</v>
+      </c>
+      <c r="C5" s="169">
+        <v>8.2191799999999995E-2</v>
+      </c>
+      <c r="D5" s="169">
+        <v>0.15068490000000001</v>
+      </c>
+      <c r="E5" s="169">
+        <v>6.1643799999999999E-2</v>
+      </c>
+      <c r="F5" s="169"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="179" t="s">
+        <v>204</v>
+      </c>
+      <c r="B6" s="169">
+        <v>4.79452E-2</v>
+      </c>
+      <c r="C6" s="169">
+        <v>4.1095899999999998E-2</v>
+      </c>
+      <c r="D6" s="169">
+        <v>2.9680399999999999E-2</v>
+      </c>
+      <c r="E6" s="169">
+        <v>4.79452E-2</v>
+      </c>
+      <c r="F6" s="169"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="179" t="s">
+        <v>201</v>
+      </c>
+      <c r="B7" s="169">
+        <v>6.8493E-3</v>
+      </c>
+      <c r="C7" s="169">
+        <v>9.1324000000000006E-3</v>
+      </c>
+      <c r="D7" s="169">
+        <v>9.1324000000000006E-3</v>
+      </c>
+      <c r="E7" s="169">
+        <v>0.34931509999999999</v>
+      </c>
+      <c r="F7" s="169"/>
+    </row>
+    <row r="8" spans="1:6" ht="19" thickBot="1">
+      <c r="A8" s="198" t="s">
+        <v>202</v>
+      </c>
+      <c r="B8" s="173">
+        <v>0.1118721</v>
+      </c>
+      <c r="C8" s="173">
+        <v>0.18036530000000001</v>
+      </c>
+      <c r="D8" s="173">
+        <v>0.1232877</v>
+      </c>
+      <c r="E8" s="169">
+        <v>9.1324000000000006E-3</v>
+      </c>
+      <c r="F8" s="169"/>
+    </row>
+    <row r="9" spans="1:6" ht="19" thickBot="1">
+      <c r="E9" s="173"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="195" t="s">
+        <v>216</v>
+      </c>
+      <c r="B10" s="165">
+        <v>2.8310499999999998</v>
+      </c>
+      <c r="C10" s="165">
+        <v>2.6392690000000001</v>
+      </c>
+      <c r="D10" s="165">
+        <v>2.8424659999999999</v>
+      </c>
+      <c r="E10" s="165">
+        <v>1.8333330000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="179" t="s">
+        <v>206</v>
+      </c>
+      <c r="B11" s="169">
+        <v>0.38584469999999998</v>
+      </c>
+      <c r="C11" s="169">
+        <v>0.31963469999999999</v>
+      </c>
+      <c r="D11" s="169">
+        <v>0.40867579999999998</v>
+      </c>
+      <c r="E11" s="169">
+        <v>0.30821920000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="179" t="s">
+        <v>219</v>
+      </c>
+      <c r="B12" s="169">
+        <v>4.3379000000000001E-2</v>
+      </c>
+      <c r="C12" s="169">
+        <v>5.25114E-2</v>
+      </c>
+      <c r="D12" s="169">
+        <v>3.4246600000000002E-2</v>
+      </c>
+      <c r="E12" s="169">
+        <v>2.7397299999999999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="179" t="s">
+        <v>220</v>
+      </c>
+      <c r="B13" s="169">
+        <v>0.3835616</v>
+      </c>
+      <c r="C13" s="169">
+        <v>0.32420090000000001</v>
+      </c>
+      <c r="D13" s="169">
+        <v>0.41552509999999998</v>
+      </c>
+      <c r="E13" s="169">
+        <v>0.2899543</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="179" t="s">
+        <v>221</v>
+      </c>
+      <c r="B14" s="169">
+        <v>0.46794520000000001</v>
+      </c>
+      <c r="C14" s="169">
+        <v>0.39481739999999999</v>
+      </c>
+      <c r="D14" s="169">
+        <v>0.36520550000000002</v>
+      </c>
+      <c r="E14" s="169">
+        <v>0.35301369999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="179" t="s">
+        <v>222</v>
+      </c>
+      <c r="B15" s="169">
+        <v>0.17123289999999999</v>
+      </c>
+      <c r="C15" s="169">
+        <v>0.1050228</v>
+      </c>
+      <c r="D15" s="169">
+        <v>0.1347032</v>
+      </c>
+      <c r="E15" s="169">
+        <v>0.10045659999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="179" t="s">
+        <v>217</v>
+      </c>
+      <c r="B16" s="169">
+        <v>1.114233</v>
+      </c>
+      <c r="C16" s="169">
+        <v>0.7416895</v>
+      </c>
+      <c r="D16" s="169">
+        <v>1.045479</v>
+      </c>
+      <c r="E16" s="169">
+        <v>0.59344750000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="179" t="s">
+        <v>218</v>
+      </c>
+      <c r="B17" s="169">
+        <v>0.32420090000000001</v>
+      </c>
+      <c r="C17" s="169">
+        <v>0.283105</v>
+      </c>
+      <c r="D17" s="169">
+        <v>0.31050230000000001</v>
+      </c>
+      <c r="E17" s="169">
+        <v>0.23287669999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="19" thickBot="1">
+      <c r="A18" s="198" t="s">
+        <v>227</v>
+      </c>
+      <c r="B18" s="173">
+        <v>0.27168949999999997</v>
+      </c>
+      <c r="C18" s="173">
+        <v>0.29452050000000002</v>
+      </c>
+      <c r="D18" s="173">
+        <v>0.26712330000000001</v>
+      </c>
+      <c r="E18" s="173">
+        <v>0.1780822</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="19" thickBot="1">
+      <c r="A20" s="176" t="s">
+        <v>224</v>
+      </c>
+      <c r="B20" s="160"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="195" t="s">
+        <v>250</v>
+      </c>
+      <c r="B21" s="165">
+        <v>2.2831000000000001E-3</v>
+      </c>
+      <c r="C21" s="165">
+        <v>2.2831000000000001E-3</v>
+      </c>
+      <c r="D21" s="165">
+        <v>2.2831000000000001E-3</v>
+      </c>
+      <c r="E21" s="165">
+        <v>4.5662000000000003E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="179" t="s">
+        <v>245</v>
+      </c>
+      <c r="B22" s="169">
+        <v>7.9908699999999999E-2</v>
+      </c>
+      <c r="C22" s="169">
+        <v>0.1666667</v>
+      </c>
+      <c r="D22" s="169">
+        <v>9.1324199999999994E-2</v>
+      </c>
+      <c r="E22" s="169">
+        <v>4.3379000000000001E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="179" t="s">
+        <v>246</v>
+      </c>
+      <c r="B23" s="169">
+        <v>0.18949769999999999</v>
+      </c>
+      <c r="C23" s="169">
+        <v>0.15296799999999999</v>
+      </c>
+      <c r="D23" s="169">
+        <v>0.16894980000000001</v>
+      </c>
+      <c r="E23" s="169">
+        <v>0.15068490000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="179" t="s">
+        <v>383</v>
+      </c>
+      <c r="B24" s="169">
+        <v>0.48401830000000001</v>
+      </c>
+      <c r="C24" s="169">
+        <v>0.50456619999999996</v>
+      </c>
+      <c r="D24" s="169">
+        <v>0.50228309999999998</v>
+      </c>
+      <c r="E24" s="169">
+        <v>0.39497719999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="179" t="s">
+        <v>248</v>
+      </c>
+      <c r="B25" s="169">
+        <v>0.24429219999999999</v>
+      </c>
+      <c r="C25" s="169">
+        <v>0.173516</v>
+      </c>
+      <c r="D25" s="169">
+        <v>0.2351598</v>
+      </c>
+      <c r="E25" s="169">
+        <v>5.7077599999999999E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="19" thickBot="1">
+      <c r="A26" s="198" t="s">
+        <v>249</v>
+      </c>
+      <c r="B26" s="173">
+        <v>0.44520549999999998</v>
+      </c>
+      <c r="C26" s="173">
+        <v>0.42922369999999999</v>
+      </c>
+      <c r="D26" s="173">
+        <v>0.45433790000000002</v>
+      </c>
+      <c r="E26" s="173">
+        <v>0.37214609999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="13"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA329E4-6CE6-BB44-AA7A-758E4F0081C1}">
   <dimension ref="A1:AW29"/>
   <sheetViews>

</xml_diff>

<commit_message>
finished the poster for IMaSS
</commit_message>
<xml_diff>
--- a/3_Toyota_Data_Modeling/STATA/1_STATA_Mode_Estimation Results.xlsx
+++ b/3_Toyota_Data_Modeling/STATA/1_STATA_Mode_Estimation Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ghasak/Desktop/Toyota_Project_Data_Wrangling/3_Toyota_Data_Modeling/STATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD5EFAA-CDDE-D343-93A4-077F5E53934F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6AB8DC-6FAC-BF46-A8D8-A5069F19CA9E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test " sheetId="1" r:id="rId1"/>
@@ -1888,10 +1888,10 @@
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="0.000"/>
     <numFmt numFmtId="177" formatCode="0.0000"/>
-    <numFmt numFmtId="180" formatCode="0.0000000"/>
-    <numFmt numFmtId="182" formatCode="0.000_ "/>
-    <numFmt numFmtId="187" formatCode="0.0000000_ "/>
-    <numFmt numFmtId="188" formatCode="0.00000000000000_ "/>
+    <numFmt numFmtId="178" formatCode="0.0000000"/>
+    <numFmt numFmtId="179" formatCode="0.000_ "/>
+    <numFmt numFmtId="180" formatCode="0.0000000_ "/>
+    <numFmt numFmtId="181" formatCode="0.00000000000000_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -4111,100 +4111,7 @@
     <xf numFmtId="0" fontId="19" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4265,29 +4172,122 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="188" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1407">
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -5698,77 +5698,7 @@
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-00007D050000}"/>
     <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-00007E050000}"/>
   </cellStyles>
-  <dxfs count="800">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="790">
     <dxf>
       <fill>
         <patternFill>
@@ -11627,7 +11557,7 @@
   <dimension ref="B1:S48"/>
   <sheetViews>
     <sheetView zoomScale="161" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:F7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18"/>
@@ -12253,42 +12183,42 @@
   </sheetData>
   <phoneticPr fontId="12"/>
   <conditionalFormatting sqref="G3">
-    <cfRule type="cellIs" dxfId="799" priority="21" operator="between">
+    <cfRule type="cellIs" dxfId="789" priority="21" operator="between">
       <formula>$F$6</formula>
       <formula>$F$7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="798" priority="22" operator="between">
+    <cfRule type="cellIs" dxfId="788" priority="22" operator="between">
       <formula>$E$6</formula>
       <formula>$E$7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="797" priority="23" operator="between">
+    <cfRule type="cellIs" dxfId="787" priority="23" operator="between">
       <formula>$F$5</formula>
       <formula>$F$6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="796" priority="24" operator="between">
+    <cfRule type="cellIs" dxfId="786" priority="24" operator="between">
       <formula>$E$5</formula>
       <formula>$E$6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="795" priority="25" operator="between">
+    <cfRule type="cellIs" dxfId="785" priority="25" operator="between">
       <formula>$F$4</formula>
       <formula>$F$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="794" priority="26" operator="between">
+    <cfRule type="cellIs" dxfId="784" priority="26" operator="between">
       <formula>$E$4</formula>
       <formula>$E$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="793" priority="27" operator="between">
+    <cfRule type="cellIs" dxfId="783" priority="27" operator="between">
       <formula>$F$3</formula>
       <formula>$F$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="792" priority="28" operator="between">
+    <cfRule type="cellIs" dxfId="782" priority="28" operator="between">
       <formula>$E$3</formula>
       <formula>$E$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="791" priority="29" operator="lessThan">
+    <cfRule type="cellIs" dxfId="781" priority="29" operator="lessThan">
       <formula>$F$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="790" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="780" priority="30" operator="greaterThan">
       <formula>$E$3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12301,7 +12231,7 @@
   <dimension ref="A1:Q37"/>
   <sheetViews>
     <sheetView zoomScale="132" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18"/>
@@ -12317,7 +12247,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="28.5" customHeight="1" thickBot="1">
-      <c r="A1" s="186" t="s">
+      <c r="A1" s="155" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="24" t="s">
@@ -12340,10 +12270,10 @@
       <c r="A2" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="179">
+      <c r="B2" s="148">
         <v>5.0276500000000004</v>
       </c>
-      <c r="C2" s="179">
+      <c r="C2" s="148">
         <v>5.5500389999999999</v>
       </c>
       <c r="D2" s="25"/>
@@ -12381,10 +12311,10 @@
       <c r="A3" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="182">
+      <c r="B3" s="151">
         <v>0.96313360000000003</v>
       </c>
-      <c r="C3" s="182">
+      <c r="C3" s="151">
         <v>1.65459</v>
       </c>
       <c r="D3" s="27"/>
@@ -12406,10 +12336,10 @@
       <c r="A4" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="182">
+      <c r="B4" s="151">
         <v>3.2949310000000001</v>
       </c>
-      <c r="C4" s="182">
+      <c r="C4" s="151">
         <v>3.6750980000000002</v>
       </c>
       <c r="D4" s="27"/>
@@ -12443,10 +12373,10 @@
       <c r="A5" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="181">
+      <c r="B5" s="150">
         <v>0.76958530000000003</v>
       </c>
-      <c r="C5" s="181">
+      <c r="C5" s="150">
         <v>1.0648260000000001</v>
       </c>
       <c r="D5" s="28"/>
@@ -12480,10 +12410,10 @@
       <c r="A6" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="182">
+      <c r="B6" s="151">
         <v>0.29953920000000001</v>
       </c>
-      <c r="C6" s="182"/>
+      <c r="C6" s="151"/>
       <c r="D6" s="26"/>
       <c r="E6" s="32"/>
       <c r="F6" s="82"/>
@@ -12515,10 +12445,10 @@
       <c r="A7" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="182">
+      <c r="B7" s="151">
         <v>0.28801840000000001</v>
       </c>
-      <c r="C7" s="182"/>
+      <c r="C7" s="151"/>
       <c r="D7" s="26"/>
       <c r="E7" s="32"/>
       <c r="F7" s="82"/>
@@ -12550,10 +12480,10 @@
       <c r="A8" s="15" t="s">
         <v>475</v>
       </c>
-      <c r="B8" s="179">
+      <c r="B8" s="148">
         <v>7.3732699999999998E-2</v>
       </c>
-      <c r="C8" s="179"/>
+      <c r="C8" s="148"/>
       <c r="D8" s="22"/>
       <c r="E8" s="17"/>
       <c r="F8" s="81"/>
@@ -12585,10 +12515,10 @@
       <c r="A9" s="13" t="s">
         <v>476</v>
       </c>
-      <c r="B9" s="182">
+      <c r="B9" s="151">
         <v>0.68433180000000005</v>
       </c>
-      <c r="C9" s="182"/>
+      <c r="C9" s="151"/>
       <c r="D9" s="21"/>
       <c r="E9" s="16"/>
       <c r="F9" s="82"/>
@@ -12608,10 +12538,10 @@
       <c r="A10" s="13" t="s">
         <v>477</v>
       </c>
-      <c r="B10" s="182">
+      <c r="B10" s="151">
         <v>0.65668199999999999</v>
       </c>
-      <c r="C10" s="182"/>
+      <c r="C10" s="151"/>
       <c r="D10" s="21"/>
       <c r="E10" s="16"/>
       <c r="F10" s="82"/>
@@ -12643,10 +12573,10 @@
       <c r="A11" s="13" t="s">
         <v>453</v>
       </c>
-      <c r="B11" s="182">
+      <c r="B11" s="151">
         <v>0.23271890000000001</v>
       </c>
-      <c r="C11" s="182"/>
+      <c r="C11" s="151"/>
       <c r="D11" s="21"/>
       <c r="E11" s="21"/>
       <c r="F11" s="79"/>
@@ -12675,13 +12605,13 @@
       <c r="Q11" s="10"/>
     </row>
     <row r="12" spans="1:17" ht="19" thickBot="1">
-      <c r="A12" s="180" t="s">
+      <c r="A12" s="149" t="s">
         <v>478</v>
       </c>
-      <c r="B12" s="181">
+      <c r="B12" s="150">
         <v>0.4447005</v>
       </c>
-      <c r="C12" s="181"/>
+      <c r="C12" s="150"/>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
       <c r="F12" s="80"/>
@@ -12713,15 +12643,15 @@
       <c r="A13" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="179">
+      <c r="B13" s="148">
         <v>2.977252</v>
       </c>
-      <c r="C13" s="179">
+      <c r="C13" s="148">
         <v>2.0887500000000001</v>
       </c>
-      <c r="D13" s="187"/>
-      <c r="E13" s="187"/>
-      <c r="F13" s="188"/>
+      <c r="D13" s="156"/>
+      <c r="E13" s="156"/>
+      <c r="F13" s="157"/>
       <c r="I13" s="10" t="s">
         <v>439</v>
       </c>
@@ -12750,7 +12680,7 @@
       <c r="A14" s="13" t="s">
         <v>454</v>
       </c>
-      <c r="B14" s="182">
+      <c r="B14" s="151">
         <v>0.35253459999999998</v>
       </c>
       <c r="C14" s="20"/>
@@ -12784,17 +12714,17 @@
       <c r="Q14" s="10"/>
     </row>
     <row r="15" spans="1:17" ht="19" thickBot="1">
-      <c r="A15" s="180" t="s">
+      <c r="A15" s="149" t="s">
         <v>470</v>
       </c>
-      <c r="B15" s="181">
+      <c r="B15" s="150">
         <v>3.180679</v>
       </c>
-      <c r="C15" s="181">
+      <c r="C15" s="150">
         <v>0.5932501</v>
       </c>
-      <c r="D15" s="184"/>
-      <c r="E15" s="184"/>
+      <c r="D15" s="153"/>
+      <c r="E15" s="153"/>
       <c r="F15" s="83" t="s">
         <v>471</v>
       </c>
@@ -12814,14 +12744,14 @@
       <c r="A16" s="15" t="s">
         <v>469</v>
       </c>
-      <c r="B16" s="179">
+      <c r="B16" s="148">
         <v>0.89182620000000001</v>
       </c>
-      <c r="C16" s="179">
+      <c r="C16" s="148">
         <v>0.70488779999999995</v>
       </c>
-      <c r="D16" s="187"/>
-      <c r="E16" s="187"/>
+      <c r="D16" s="156"/>
+      <c r="E16" s="156"/>
       <c r="F16" s="81" t="s">
         <v>472</v>
       </c>
@@ -12853,15 +12783,15 @@
       <c r="A17" s="13" t="s">
         <v>460</v>
       </c>
-      <c r="B17" s="182">
+      <c r="B17" s="151">
         <v>2.2506620000000002</v>
       </c>
-      <c r="C17" s="182">
+      <c r="C17" s="151">
         <v>0.36256850000000002</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="20"/>
-      <c r="F17" s="183"/>
+      <c r="F17" s="152"/>
       <c r="I17" s="10" t="s">
         <v>442</v>
       </c>
@@ -12890,7 +12820,7 @@
       <c r="A18" s="13" t="s">
         <v>461</v>
       </c>
-      <c r="B18" s="182">
+      <c r="B18" s="151">
         <v>0.55529949999999995</v>
       </c>
       <c r="C18" s="20"/>
@@ -12926,10 +12856,10 @@
       <c r="A19" s="13" t="s">
         <v>473</v>
       </c>
-      <c r="B19" s="182">
+      <c r="B19" s="151">
         <v>0.6336406</v>
       </c>
-      <c r="C19" s="182"/>
+      <c r="C19" s="151"/>
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
       <c r="F19" s="82" t="s">
@@ -12944,10 +12874,10 @@
       <c r="A20" s="13" t="s">
         <v>479</v>
       </c>
-      <c r="B20" s="182">
+      <c r="B20" s="151">
         <v>0.36866359999999998</v>
       </c>
-      <c r="C20" s="182"/>
+      <c r="C20" s="151"/>
       <c r="D20" s="20"/>
       <c r="E20" s="20"/>
       <c r="F20" s="82"/>
@@ -12959,10 +12889,10 @@
       <c r="A21" s="13" t="s">
         <v>462</v>
       </c>
-      <c r="B21" s="182">
+      <c r="B21" s="151">
         <v>8.6539900000000003E-2</v>
       </c>
-      <c r="C21" s="182">
+      <c r="C21" s="151">
         <v>0.3017608</v>
       </c>
       <c r="D21" s="20"/>
@@ -12998,10 +12928,10 @@
       <c r="A22" s="13" t="s">
         <v>463</v>
       </c>
-      <c r="B22" s="182">
+      <c r="B22" s="151">
         <v>0.53456219999999999</v>
       </c>
-      <c r="C22" s="182"/>
+      <c r="C22" s="151"/>
       <c r="D22" s="20"/>
       <c r="E22" s="20"/>
       <c r="F22" s="82" t="s">
@@ -13037,10 +12967,10 @@
       <c r="A23" s="13" t="s">
         <v>474</v>
       </c>
-      <c r="B23" s="182">
+      <c r="B23" s="151">
         <v>0.2050691</v>
       </c>
-      <c r="C23" s="182"/>
+      <c r="C23" s="151"/>
       <c r="D23" s="20"/>
       <c r="E23" s="20"/>
       <c r="F23" s="82" t="s">
@@ -13061,15 +12991,15 @@
       <c r="Q23" s="10"/>
     </row>
     <row r="24" spans="1:17" ht="19" thickBot="1">
-      <c r="A24" s="180" t="s">
+      <c r="A24" s="149" t="s">
         <v>467</v>
       </c>
-      <c r="B24" s="181">
+      <c r="B24" s="150">
         <v>0.53686639999999997</v>
       </c>
-      <c r="C24" s="181"/>
-      <c r="D24" s="184"/>
-      <c r="E24" s="184"/>
+      <c r="C24" s="150"/>
+      <c r="D24" s="153"/>
+      <c r="E24" s="153"/>
       <c r="F24" s="83" t="s">
         <v>468</v>
       </c>
@@ -13677,7 +13607,7 @@
       <c r="G16" s="97">
         <v>1</v>
       </c>
-      <c r="H16" s="149" t="s">
+      <c r="H16" s="188" t="s">
         <v>81</v>
       </c>
       <c r="I16" s="110" t="s">
@@ -13703,7 +13633,7 @@
       <c r="G17" s="101">
         <v>1</v>
       </c>
-      <c r="H17" s="150"/>
+      <c r="H17" s="189"/>
       <c r="I17" s="113" t="s">
         <v>70</v>
       </c>
@@ -13727,7 +13657,7 @@
       <c r="G18" s="101">
         <v>1</v>
       </c>
-      <c r="H18" s="150"/>
+      <c r="H18" s="189"/>
       <c r="I18" s="113" t="s">
         <v>71</v>
       </c>
@@ -13751,7 +13681,7 @@
       <c r="G19" s="101">
         <v>1</v>
       </c>
-      <c r="H19" s="150"/>
+      <c r="H19" s="189"/>
       <c r="I19" s="113" t="s">
         <v>72</v>
       </c>
@@ -13775,7 +13705,7 @@
       <c r="G20" s="101">
         <v>1</v>
       </c>
-      <c r="H20" s="150"/>
+      <c r="H20" s="189"/>
       <c r="I20" s="113" t="s">
         <v>73</v>
       </c>
@@ -13799,7 +13729,7 @@
       <c r="G21" s="105">
         <v>1</v>
       </c>
-      <c r="H21" s="151"/>
+      <c r="H21" s="190"/>
       <c r="I21" s="115" t="s">
         <v>74</v>
       </c>
@@ -13828,7 +13758,7 @@
       <c r="G23" s="97">
         <v>1</v>
       </c>
-      <c r="H23" s="146" t="s">
+      <c r="H23" s="185" t="s">
         <v>86</v>
       </c>
       <c r="I23" s="110"/>
@@ -13849,7 +13779,7 @@
       <c r="G24" s="101">
         <v>1</v>
       </c>
-      <c r="H24" s="147"/>
+      <c r="H24" s="186"/>
       <c r="I24" s="113"/>
     </row>
     <row r="25" spans="3:12">
@@ -13868,7 +13798,7 @@
       <c r="G25" s="101">
         <v>1</v>
       </c>
-      <c r="H25" s="147"/>
+      <c r="H25" s="186"/>
       <c r="I25" s="113"/>
     </row>
     <row r="26" spans="3:12" ht="16" thickBot="1">
@@ -13887,7 +13817,7 @@
       <c r="G26" s="105">
         <v>1</v>
       </c>
-      <c r="H26" s="148"/>
+      <c r="H26" s="187"/>
       <c r="I26" s="115"/>
     </row>
     <row r="27" spans="3:12" ht="17" thickBot="1">
@@ -13911,7 +13841,7 @@
       <c r="G28" s="97">
         <v>1</v>
       </c>
-      <c r="H28" s="146" t="s">
+      <c r="H28" s="185" t="s">
         <v>96</v>
       </c>
       <c r="I28" s="110" t="s">
@@ -13934,7 +13864,7 @@
       <c r="G29" s="101">
         <v>1</v>
       </c>
-      <c r="H29" s="147"/>
+      <c r="H29" s="186"/>
       <c r="I29" s="113" t="s">
         <v>89</v>
       </c>
@@ -13955,7 +13885,7 @@
       <c r="G30" s="101">
         <v>1</v>
       </c>
-      <c r="H30" s="147"/>
+      <c r="H30" s="186"/>
       <c r="I30" s="113" t="s">
         <v>90</v>
       </c>
@@ -13976,7 +13906,7 @@
       <c r="G31" s="105">
         <v>1</v>
       </c>
-      <c r="H31" s="148"/>
+      <c r="H31" s="187"/>
       <c r="I31" s="115" t="s">
         <v>91</v>
       </c>
@@ -14002,7 +13932,7 @@
       <c r="G33" s="97">
         <v>1</v>
       </c>
-      <c r="H33" s="146" t="s">
+      <c r="H33" s="185" t="s">
         <v>108</v>
       </c>
       <c r="I33" s="110" t="s">
@@ -14025,7 +13955,7 @@
       <c r="G34" s="101">
         <v>1</v>
       </c>
-      <c r="H34" s="147"/>
+      <c r="H34" s="186"/>
       <c r="I34" s="113" t="s">
         <v>101</v>
       </c>
@@ -14046,7 +13976,7 @@
       <c r="G35" s="101">
         <v>1</v>
       </c>
-      <c r="H35" s="147"/>
+      <c r="H35" s="186"/>
       <c r="I35" s="113" t="s">
         <v>102</v>
       </c>
@@ -14067,7 +13997,7 @@
       <c r="G36" s="105">
         <v>1</v>
       </c>
-      <c r="H36" s="148"/>
+      <c r="H36" s="187"/>
       <c r="I36" s="115" t="s">
         <v>103</v>
       </c>
@@ -14093,7 +14023,7 @@
       <c r="G38" s="97">
         <v>1</v>
       </c>
-      <c r="H38" s="146" t="s">
+      <c r="H38" s="185" t="s">
         <v>116</v>
       </c>
       <c r="I38" s="110" t="s">
@@ -14116,7 +14046,7 @@
       <c r="G39" s="101">
         <v>1</v>
       </c>
-      <c r="H39" s="147"/>
+      <c r="H39" s="186"/>
       <c r="I39" s="113" t="s">
         <v>38</v>
       </c>
@@ -14137,7 +14067,7 @@
       <c r="G40" s="101">
         <v>1</v>
       </c>
-      <c r="H40" s="147"/>
+      <c r="H40" s="186"/>
       <c r="I40" s="113" t="s">
         <v>39</v>
       </c>
@@ -14158,7 +14088,7 @@
       <c r="G41" s="101">
         <v>1</v>
       </c>
-      <c r="H41" s="147"/>
+      <c r="H41" s="186"/>
       <c r="I41" s="113" t="s">
         <v>115</v>
       </c>
@@ -14179,7 +14109,7 @@
       <c r="G42" s="105">
         <v>1</v>
       </c>
-      <c r="H42" s="148"/>
+      <c r="H42" s="187"/>
       <c r="I42" s="115" t="s">
         <v>40</v>
       </c>
@@ -14205,7 +14135,7 @@
       <c r="G44" s="97">
         <v>1</v>
       </c>
-      <c r="H44" s="149" t="s">
+      <c r="H44" s="188" t="s">
         <v>123</v>
       </c>
       <c r="I44" s="110" t="s">
@@ -14228,7 +14158,7 @@
       <c r="G45" s="101">
         <v>1</v>
       </c>
-      <c r="H45" s="150"/>
+      <c r="H45" s="189"/>
       <c r="I45" s="113" t="s">
         <v>118</v>
       </c>
@@ -14249,7 +14179,7 @@
       <c r="G46" s="101">
         <v>1</v>
       </c>
-      <c r="H46" s="150"/>
+      <c r="H46" s="189"/>
       <c r="I46" s="113" t="s">
         <v>119</v>
       </c>
@@ -14270,7 +14200,7 @@
       <c r="G47" s="105">
         <v>1</v>
       </c>
-      <c r="H47" s="151"/>
+      <c r="H47" s="190"/>
       <c r="I47" s="115" t="s">
         <v>120</v>
       </c>
@@ -14390,7 +14320,7 @@
       <c r="G56" s="97">
         <v>1</v>
       </c>
-      <c r="H56" s="146" t="s">
+      <c r="H56" s="185" t="s">
         <v>139</v>
       </c>
       <c r="I56" s="110" t="s">
@@ -14413,7 +14343,7 @@
       <c r="G57" s="101">
         <v>1</v>
       </c>
-      <c r="H57" s="147"/>
+      <c r="H57" s="186"/>
       <c r="I57" s="113" t="s">
         <v>135</v>
       </c>
@@ -14434,7 +14364,7 @@
       <c r="G58" s="101">
         <v>1</v>
       </c>
-      <c r="H58" s="147"/>
+      <c r="H58" s="186"/>
       <c r="I58" s="113" t="s">
         <v>131</v>
       </c>
@@ -14455,7 +14385,7 @@
       <c r="G59" s="101">
         <v>1</v>
       </c>
-      <c r="H59" s="147"/>
+      <c r="H59" s="186"/>
       <c r="I59" s="113" t="s">
         <v>132</v>
       </c>
@@ -14476,7 +14406,7 @@
       <c r="G60" s="105">
         <v>1</v>
       </c>
-      <c r="H60" s="148"/>
+      <c r="H60" s="187"/>
       <c r="I60" s="115" t="s">
         <v>133</v>
       </c>
@@ -14591,7 +14521,7 @@
       <c r="G67" s="97">
         <v>38.51</v>
       </c>
-      <c r="H67" s="146" t="s">
+      <c r="H67" s="185" t="s">
         <v>166</v>
       </c>
       <c r="I67" s="110" t="s">
@@ -14614,7 +14544,7 @@
       <c r="G68" s="101">
         <v>141.63</v>
       </c>
-      <c r="H68" s="147"/>
+      <c r="H68" s="186"/>
       <c r="I68" s="113" t="s">
         <v>154</v>
       </c>
@@ -14635,7 +14565,7 @@
       <c r="G69" s="101">
         <v>51.61</v>
       </c>
-      <c r="H69" s="147"/>
+      <c r="H69" s="186"/>
       <c r="I69" s="113" t="s">
         <v>155</v>
       </c>
@@ -14656,7 +14586,7 @@
       <c r="G70" s="101">
         <v>28.03</v>
       </c>
-      <c r="H70" s="147"/>
+      <c r="H70" s="186"/>
       <c r="I70" s="113" t="s">
         <v>156</v>
       </c>
@@ -14677,7 +14607,7 @@
       <c r="G71" s="101">
         <v>16.53</v>
       </c>
-      <c r="H71" s="147"/>
+      <c r="H71" s="186"/>
       <c r="I71" s="113" t="s">
         <v>157</v>
       </c>
@@ -14698,7 +14628,7 @@
       <c r="G72" s="105">
         <v>2.5299999999999998</v>
       </c>
-      <c r="H72" s="148"/>
+      <c r="H72" s="187"/>
       <c r="I72" s="115" t="s">
         <v>158</v>
       </c>
@@ -18267,10 +18197,10 @@
   <dimension ref="A1:Y131"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="N5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="W16" sqref="W16"/>
+      <selection pane="bottomRight" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="18"/>
@@ -18302,115 +18232,115 @@
   <sheetData>
     <row r="1" spans="1:25" s="11" customFormat="1" ht="41" thickBot="1">
       <c r="A1" s="12"/>
-      <c r="B1" s="170" t="s">
+      <c r="B1" s="194" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="171"/>
-      <c r="D1" s="171"/>
-      <c r="E1" s="171"/>
-      <c r="F1" s="171"/>
-      <c r="G1" s="171"/>
-      <c r="H1" s="171"/>
-      <c r="I1" s="171"/>
-      <c r="J1" s="171"/>
-      <c r="K1" s="171"/>
-      <c r="L1" s="171"/>
-      <c r="M1" s="171"/>
-      <c r="N1" s="171"/>
-      <c r="O1" s="171"/>
-      <c r="P1" s="171"/>
-      <c r="Q1" s="171"/>
-      <c r="R1" s="171"/>
-      <c r="S1" s="171"/>
-      <c r="T1" s="171"/>
-      <c r="U1" s="171"/>
-      <c r="V1" s="171"/>
-      <c r="W1" s="171"/>
-      <c r="X1" s="171"/>
-      <c r="Y1" s="171"/>
+      <c r="C1" s="195"/>
+      <c r="D1" s="195"/>
+      <c r="E1" s="195"/>
+      <c r="F1" s="195"/>
+      <c r="G1" s="195"/>
+      <c r="H1" s="195"/>
+      <c r="I1" s="195"/>
+      <c r="J1" s="195"/>
+      <c r="K1" s="195"/>
+      <c r="L1" s="195"/>
+      <c r="M1" s="195"/>
+      <c r="N1" s="195"/>
+      <c r="O1" s="195"/>
+      <c r="P1" s="195"/>
+      <c r="Q1" s="195"/>
+      <c r="R1" s="195"/>
+      <c r="S1" s="195"/>
+      <c r="T1" s="195"/>
+      <c r="U1" s="195"/>
+      <c r="V1" s="195"/>
+      <c r="W1" s="195"/>
+      <c r="X1" s="195"/>
+      <c r="Y1" s="195"/>
     </row>
     <row r="2" spans="1:25" ht="19" thickBot="1">
-      <c r="A2" s="152" t="s">
+      <c r="A2" s="201" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="168" t="s">
+      <c r="B2" s="217" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="169"/>
-      <c r="D2" s="169"/>
-      <c r="E2" s="169"/>
-      <c r="F2" s="169"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="166" t="s">
+      <c r="C2" s="218"/>
+      <c r="D2" s="218"/>
+      <c r="E2" s="218"/>
+      <c r="F2" s="218"/>
+      <c r="G2" s="218"/>
+      <c r="H2" s="212" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="167"/>
-      <c r="J2" s="167"/>
-      <c r="K2" s="167"/>
-      <c r="L2" s="167"/>
-      <c r="M2" s="167"/>
-      <c r="N2" s="158" t="s">
+      <c r="I2" s="213"/>
+      <c r="J2" s="213"/>
+      <c r="K2" s="213"/>
+      <c r="L2" s="213"/>
+      <c r="M2" s="213"/>
+      <c r="N2" s="207" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="159"/>
-      <c r="P2" s="159"/>
-      <c r="Q2" s="159"/>
-      <c r="R2" s="159"/>
-      <c r="S2" s="159"/>
-      <c r="T2" s="172" t="s">
+      <c r="O2" s="208"/>
+      <c r="P2" s="208"/>
+      <c r="Q2" s="208"/>
+      <c r="R2" s="208"/>
+      <c r="S2" s="208"/>
+      <c r="T2" s="196" t="s">
         <v>50</v>
       </c>
-      <c r="U2" s="173"/>
-      <c r="V2" s="173"/>
-      <c r="W2" s="173"/>
-      <c r="X2" s="173"/>
-      <c r="Y2" s="173"/>
+      <c r="U2" s="197"/>
+      <c r="V2" s="197"/>
+      <c r="W2" s="197"/>
+      <c r="X2" s="197"/>
+      <c r="Y2" s="197"/>
     </row>
     <row r="3" spans="1:25" ht="19" thickBot="1">
-      <c r="A3" s="153"/>
-      <c r="B3" s="155" t="s">
+      <c r="A3" s="202"/>
+      <c r="B3" s="204" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="156"/>
-      <c r="D3" s="156"/>
-      <c r="E3" s="155" t="s">
+      <c r="C3" s="205"/>
+      <c r="D3" s="205"/>
+      <c r="E3" s="204" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="156"/>
-      <c r="G3" s="157"/>
-      <c r="H3" s="165" t="s">
+      <c r="F3" s="205"/>
+      <c r="G3" s="206"/>
+      <c r="H3" s="215" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="163"/>
-      <c r="J3" s="164"/>
-      <c r="K3" s="163" t="s">
+      <c r="I3" s="214"/>
+      <c r="J3" s="216"/>
+      <c r="K3" s="214" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="163"/>
-      <c r="M3" s="163"/>
-      <c r="N3" s="160" t="s">
+      <c r="L3" s="214"/>
+      <c r="M3" s="214"/>
+      <c r="N3" s="209" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="161"/>
-      <c r="P3" s="161"/>
-      <c r="Q3" s="160" t="s">
+      <c r="O3" s="210"/>
+      <c r="P3" s="210"/>
+      <c r="Q3" s="209" t="s">
         <v>34</v>
       </c>
-      <c r="R3" s="161"/>
-      <c r="S3" s="162"/>
-      <c r="T3" s="174" t="s">
+      <c r="R3" s="210"/>
+      <c r="S3" s="211"/>
+      <c r="T3" s="198" t="s">
         <v>24</v>
       </c>
-      <c r="U3" s="175"/>
-      <c r="V3" s="175"/>
-      <c r="W3" s="174" t="s">
+      <c r="U3" s="199"/>
+      <c r="V3" s="199"/>
+      <c r="W3" s="198" t="s">
         <v>34</v>
       </c>
-      <c r="X3" s="175"/>
-      <c r="Y3" s="176"/>
+      <c r="X3" s="199"/>
+      <c r="Y3" s="200"/>
     </row>
     <row r="4" spans="1:25" ht="20" thickBot="1">
-      <c r="A4" s="154"/>
+      <c r="A4" s="203"/>
       <c r="B4" s="67" t="s">
         <v>20</v>
       </c>
@@ -18488,60 +18418,60 @@
       <c r="A5" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="178">
+      <c r="B5" s="147">
         <v>2.5283699999999999E-2</v>
       </c>
-      <c r="C5" s="178">
+      <c r="C5" s="147">
         <v>0.12230480000000001</v>
       </c>
       <c r="D5" s="39">
         <f t="shared" ref="D5:D17" si="0">B5/C5</f>
         <v>0.20672696410933994</v>
       </c>
-      <c r="E5" s="178">
+      <c r="E5" s="147">
         <v>4.1941399999999997E-2</v>
       </c>
-      <c r="F5" s="178">
+      <c r="F5" s="147">
         <v>0.13194690000000001</v>
       </c>
       <c r="G5" s="40">
         <f t="shared" ref="G5:G23" si="1">E5/F5</f>
         <v>0.31786574750903579</v>
       </c>
-      <c r="H5" s="178">
+      <c r="H5" s="147">
         <v>0.1987631</v>
       </c>
-      <c r="I5" s="178">
+      <c r="I5" s="147">
         <v>6.4143599999999995E-2</v>
       </c>
       <c r="J5" s="40">
         <f t="shared" ref="J5:J23" si="2">H5/I5</f>
         <v>3.0987206829675915</v>
       </c>
-      <c r="K5" s="178">
+      <c r="K5" s="147">
         <v>0.20470079999999999</v>
       </c>
-      <c r="L5" s="178">
+      <c r="L5" s="147">
         <v>6.7503999999999995E-2</v>
       </c>
       <c r="M5" s="39">
         <f t="shared" ref="M5:M23" si="3">K5/L5</f>
         <v>3.0324247452002844</v>
       </c>
-      <c r="N5" s="178">
+      <c r="N5" s="147">
         <v>0.2170425</v>
       </c>
-      <c r="O5" s="178">
+      <c r="O5" s="147">
         <v>0.1322796</v>
       </c>
       <c r="P5" s="39">
         <f t="shared" ref="P5:P23" si="4">N5/O5</f>
         <v>1.6407858808160896</v>
       </c>
-      <c r="Q5" s="178">
+      <c r="Q5" s="147">
         <v>0.2179613</v>
       </c>
-      <c r="R5" s="178">
+      <c r="R5" s="147">
         <v>0.13348280000000001</v>
       </c>
       <c r="S5" s="40">
@@ -18558,10 +18488,10 @@
         <f t="shared" ref="V5:V23" si="6">T5/U5</f>
         <v>3.3073304481062338</v>
       </c>
-      <c r="W5" s="178">
+      <c r="W5" s="147">
         <v>0.18261859999999999</v>
       </c>
-      <c r="X5" s="178">
+      <c r="X5" s="147">
         <v>5.8062200000000001E-2</v>
       </c>
       <c r="Y5" s="40">
@@ -18573,60 +18503,60 @@
       <c r="A6" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="178">
+      <c r="B6" s="147">
         <v>0.54355430000000005</v>
       </c>
-      <c r="C6" s="178">
+      <c r="C6" s="147">
         <v>0.17207710000000001</v>
       </c>
       <c r="D6" s="39">
         <f t="shared" si="0"/>
         <v>3.1587834755467172</v>
       </c>
-      <c r="E6" s="178">
+      <c r="E6" s="147">
         <v>0.51984059999999999</v>
       </c>
-      <c r="F6" s="178">
+      <c r="F6" s="147">
         <v>0.1894692</v>
       </c>
       <c r="G6" s="40">
         <f t="shared" si="1"/>
         <v>2.7436681001450367</v>
       </c>
-      <c r="H6" s="178">
+      <c r="H6" s="147">
         <v>0.49839319999999998</v>
       </c>
-      <c r="I6" s="178">
+      <c r="I6" s="147">
         <v>9.2792899999999998E-2</v>
       </c>
       <c r="J6" s="40">
         <f t="shared" si="2"/>
         <v>5.371027309201458</v>
       </c>
-      <c r="K6" s="178">
+      <c r="K6" s="147">
         <v>0.49068990000000001</v>
       </c>
-      <c r="L6" s="178">
+      <c r="L6" s="147">
         <v>9.8254099999999997E-2</v>
       </c>
       <c r="M6" s="39">
         <f t="shared" si="3"/>
         <v>4.9940908318329722</v>
       </c>
-      <c r="N6" s="178">
+      <c r="N6" s="147">
         <v>0.57485359999999996</v>
       </c>
-      <c r="O6" s="178">
+      <c r="O6" s="147">
         <v>0.1908386</v>
       </c>
       <c r="P6" s="39">
         <f t="shared" si="4"/>
         <v>3.012250142266816</v>
       </c>
-      <c r="Q6" s="178">
+      <c r="Q6" s="147">
         <v>0.57328299999999999</v>
       </c>
-      <c r="R6" s="178">
+      <c r="R6" s="147">
         <v>0.19243650000000001</v>
       </c>
       <c r="S6" s="40">
@@ -18643,10 +18573,10 @@
         <f t="shared" si="6"/>
         <v>7.0264858036092654</v>
       </c>
-      <c r="W6" s="178">
+      <c r="W6" s="147">
         <v>0.50424190000000002</v>
       </c>
-      <c r="X6" s="178">
+      <c r="X6" s="147">
         <v>8.4931099999999995E-2</v>
       </c>
       <c r="Y6" s="40">
@@ -18658,60 +18588,60 @@
       <c r="A7" s="15" t="s">
         <v>475</v>
       </c>
-      <c r="B7" s="178">
+      <c r="B7" s="147">
         <v>0.60978379999999999</v>
       </c>
-      <c r="C7" s="178">
+      <c r="C7" s="147">
         <v>0.15793389999999999</v>
       </c>
       <c r="D7" s="41">
         <f t="shared" si="0"/>
         <v>3.8610064083771758</v>
       </c>
-      <c r="E7" s="178">
+      <c r="E7" s="147">
         <v>0.61202279999999998</v>
       </c>
-      <c r="F7" s="178">
+      <c r="F7" s="147">
         <v>0.17111399999999999</v>
       </c>
       <c r="G7" s="42">
         <f t="shared" si="1"/>
         <v>3.5766962375959888</v>
       </c>
-      <c r="H7" s="178">
+      <c r="H7" s="147">
         <v>0.32340020000000003</v>
       </c>
-      <c r="I7" s="178">
+      <c r="I7" s="147">
         <v>8.93066E-2</v>
       </c>
       <c r="J7" s="42">
         <f t="shared" si="2"/>
         <v>3.6212351606712163</v>
       </c>
-      <c r="K7" s="178">
+      <c r="K7" s="147">
         <v>0.32236599999999999</v>
       </c>
-      <c r="L7" s="178">
+      <c r="L7" s="147">
         <v>9.3870400000000007E-2</v>
       </c>
       <c r="M7" s="41">
         <f t="shared" si="3"/>
         <v>3.4341602890794114</v>
       </c>
-      <c r="N7" s="178">
+      <c r="N7" s="147">
         <v>0.43268770000000001</v>
       </c>
-      <c r="O7" s="178">
+      <c r="O7" s="147">
         <v>0.18832779999999999</v>
       </c>
       <c r="P7" s="41">
         <f t="shared" si="4"/>
         <v>2.2975243166436394</v>
       </c>
-      <c r="Q7" s="178">
+      <c r="Q7" s="147">
         <v>0.43716389999999999</v>
       </c>
-      <c r="R7" s="178">
+      <c r="R7" s="147">
         <v>0.19023760000000001</v>
       </c>
       <c r="S7" s="42">
@@ -18728,10 +18658,10 @@
         <f t="shared" si="6"/>
         <v>5.4311275293106265</v>
       </c>
-      <c r="W7" s="178">
+      <c r="W7" s="147">
         <v>0.39115689999999997</v>
       </c>
-      <c r="X7" s="178">
+      <c r="X7" s="147">
         <v>7.9699699999999998E-2</v>
       </c>
       <c r="Y7" s="42">
@@ -18743,60 +18673,60 @@
       <c r="A8" s="13" t="s">
         <v>476</v>
       </c>
-      <c r="B8" s="178">
+      <c r="B8" s="147">
         <v>0.1528825</v>
       </c>
-      <c r="C8" s="178">
+      <c r="C8" s="147">
         <v>0.1274528</v>
       </c>
       <c r="D8" s="35">
         <f t="shared" si="0"/>
         <v>1.1995224898942982</v>
       </c>
-      <c r="E8" s="178">
+      <c r="E8" s="147">
         <v>0.1853804</v>
       </c>
-      <c r="F8" s="178">
+      <c r="F8" s="147">
         <v>0.1402158</v>
       </c>
       <c r="G8" s="36">
         <f t="shared" si="1"/>
         <v>1.322107779579762</v>
       </c>
-      <c r="H8" s="178">
+      <c r="H8" s="147">
         <v>0.69623849999999998</v>
       </c>
-      <c r="I8" s="178">
+      <c r="I8" s="147">
         <v>7.5287000000000007E-2</v>
       </c>
       <c r="J8" s="36">
         <f t="shared" si="2"/>
         <v>9.2477917834420271</v>
       </c>
-      <c r="K8" s="178">
+      <c r="K8" s="147">
         <v>0.68929870000000004</v>
       </c>
-      <c r="L8" s="178">
+      <c r="L8" s="147">
         <v>7.9028299999999996E-2</v>
       </c>
       <c r="M8" s="35">
         <f t="shared" si="3"/>
         <v>8.7221754738492425</v>
       </c>
-      <c r="N8" s="178">
+      <c r="N8" s="147">
         <v>0.72487550000000001</v>
       </c>
-      <c r="O8" s="178">
+      <c r="O8" s="147">
         <v>0.1511981</v>
       </c>
       <c r="P8" s="35">
         <f t="shared" si="4"/>
         <v>4.7942103769822504</v>
       </c>
-      <c r="Q8" s="178">
+      <c r="Q8" s="147">
         <v>0.72637339999999995</v>
       </c>
-      <c r="R8" s="178">
+      <c r="R8" s="147">
         <v>0.15257999999999999</v>
       </c>
       <c r="S8" s="36">
@@ -18813,10 +18743,10 @@
         <f t="shared" si="6"/>
         <v>10.014557161412489</v>
       </c>
-      <c r="W8" s="178">
+      <c r="W8" s="147">
         <v>0.5937907</v>
       </c>
-      <c r="X8" s="178">
+      <c r="X8" s="147">
         <v>6.5972199999999995E-2</v>
       </c>
       <c r="Y8" s="36">
@@ -18828,60 +18758,60 @@
       <c r="A9" s="13" t="s">
         <v>477</v>
       </c>
-      <c r="B9" s="178">
+      <c r="B9" s="147">
         <v>0.70616820000000002</v>
       </c>
-      <c r="C9" s="178">
+      <c r="C9" s="147">
         <v>0.16148789999999999</v>
       </c>
       <c r="D9" s="39">
         <f t="shared" si="0"/>
         <v>4.3728861419338543</v>
       </c>
-      <c r="E9" s="178">
+      <c r="E9" s="147">
         <v>0.70699279999999998</v>
       </c>
-      <c r="F9" s="178">
+      <c r="F9" s="147">
         <v>0.17256959999999999</v>
       </c>
       <c r="G9" s="40">
         <f t="shared" si="1"/>
         <v>4.0968559931760868</v>
       </c>
-      <c r="H9" s="178">
+      <c r="H9" s="147">
         <v>0.57620309999999997</v>
       </c>
-      <c r="I9" s="178">
+      <c r="I9" s="147">
         <v>7.8951300000000002E-2</v>
       </c>
       <c r="J9" s="40">
         <f t="shared" si="2"/>
         <v>7.2982091491843697</v>
       </c>
-      <c r="K9" s="178">
+      <c r="K9" s="147">
         <v>0.56979469999999999</v>
       </c>
-      <c r="L9" s="178">
+      <c r="L9" s="147">
         <v>8.2683800000000002E-2</v>
       </c>
       <c r="M9" s="39">
         <f t="shared" si="3"/>
         <v>6.8912495555356665</v>
       </c>
-      <c r="N9" s="178">
+      <c r="N9" s="147">
         <v>0.67797090000000004</v>
       </c>
-      <c r="O9" s="178">
+      <c r="O9" s="147">
         <v>0.1605125</v>
       </c>
       <c r="P9" s="39">
         <f t="shared" si="4"/>
         <v>4.2237888014952105</v>
       </c>
-      <c r="Q9" s="178">
+      <c r="Q9" s="147">
         <v>0.67597700000000005</v>
       </c>
-      <c r="R9" s="178">
+      <c r="R9" s="147">
         <v>0.1617198</v>
       </c>
       <c r="S9" s="40">
@@ -18898,10 +18828,10 @@
         <f t="shared" si="6"/>
         <v>9.328035510400202</v>
       </c>
-      <c r="W9" s="178">
+      <c r="W9" s="147">
         <v>0.59294809999999998</v>
       </c>
-      <c r="X9" s="178">
+      <c r="X9" s="147">
         <v>7.1232799999999999E-2</v>
       </c>
       <c r="Y9" s="40">
@@ -18913,60 +18843,60 @@
       <c r="A10" s="13" t="s">
         <v>453</v>
       </c>
-      <c r="B10" s="178">
+      <c r="B10" s="147">
         <v>0.23823749999999999</v>
       </c>
-      <c r="C10" s="178">
+      <c r="C10" s="147">
         <v>0.123094</v>
       </c>
       <c r="D10" s="39">
         <f t="shared" si="0"/>
         <v>1.9354111492030481</v>
       </c>
-      <c r="E10" s="178">
+      <c r="E10" s="147">
         <v>0.25379109999999999</v>
       </c>
-      <c r="F10" s="178">
+      <c r="F10" s="147">
         <v>0.13336809999999999</v>
       </c>
       <c r="G10" s="40">
         <f t="shared" si="1"/>
         <v>1.9029370591618235</v>
       </c>
-      <c r="H10" s="178">
+      <c r="H10" s="147">
         <v>0.3669615</v>
       </c>
-      <c r="I10" s="178">
+      <c r="I10" s="147">
         <v>6.6752599999999995E-2</v>
       </c>
       <c r="J10" s="40">
         <f t="shared" si="2"/>
         <v>5.4973364333374279</v>
       </c>
-      <c r="K10" s="178">
+      <c r="K10" s="147">
         <v>0.36277389999999998</v>
       </c>
-      <c r="L10" s="178">
+      <c r="L10" s="147">
         <v>7.0260799999999998E-2</v>
       </c>
       <c r="M10" s="39">
         <f t="shared" si="3"/>
         <v>5.1632475007400993</v>
       </c>
-      <c r="N10" s="178">
+      <c r="N10" s="147">
         <v>0.3133668</v>
       </c>
-      <c r="O10" s="178">
+      <c r="O10" s="147">
         <v>0.14022109999999999</v>
       </c>
       <c r="P10" s="39">
         <f t="shared" si="4"/>
         <v>2.2348048902768558</v>
       </c>
-      <c r="Q10" s="178">
+      <c r="Q10" s="147">
         <v>0.31302750000000001</v>
       </c>
-      <c r="R10" s="178">
+      <c r="R10" s="147">
         <v>0.14128769999999999</v>
       </c>
       <c r="S10" s="40">
@@ -18983,10 +18913,10 @@
         <f t="shared" si="6"/>
         <v>6.0870512834745014</v>
       </c>
-      <c r="W10" s="178">
+      <c r="W10" s="147">
         <v>0.32502399999999998</v>
       </c>
-      <c r="X10" s="178">
+      <c r="X10" s="147">
         <v>6.0291999999999998E-2</v>
       </c>
       <c r="Y10" s="40">
@@ -18995,63 +18925,63 @@
       </c>
     </row>
     <row r="11" spans="1:25" ht="19" thickBot="1">
-      <c r="A11" s="180" t="s">
+      <c r="A11" s="149" t="s">
         <v>478</v>
       </c>
-      <c r="B11" s="178">
+      <c r="B11" s="147">
         <v>0.42817820000000001</v>
       </c>
-      <c r="C11" s="178">
+      <c r="C11" s="147">
         <v>0.11929380000000001</v>
       </c>
       <c r="D11" s="41">
         <f t="shared" si="0"/>
         <v>3.5892745473779861</v>
       </c>
-      <c r="E11" s="178">
+      <c r="E11" s="147">
         <v>0.4024528</v>
       </c>
-      <c r="F11" s="178">
+      <c r="F11" s="147">
         <v>0.12909770000000001</v>
       </c>
       <c r="G11" s="42">
         <f t="shared" si="1"/>
         <v>3.1174281183940531</v>
       </c>
-      <c r="H11" s="178">
+      <c r="H11" s="147">
         <v>0.43960460000000001</v>
       </c>
-      <c r="I11" s="178">
+      <c r="I11" s="147">
         <v>6.2968399999999994E-2</v>
       </c>
       <c r="J11" s="42">
         <f t="shared" si="2"/>
         <v>6.9813525514385004</v>
       </c>
-      <c r="K11" s="178">
+      <c r="K11" s="147">
         <v>0.44187209999999999</v>
       </c>
-      <c r="L11" s="178">
+      <c r="L11" s="147">
         <v>6.6040199999999993E-2</v>
       </c>
       <c r="M11" s="41">
         <f t="shared" si="3"/>
         <v>6.6909564174548235</v>
       </c>
-      <c r="N11" s="178">
+      <c r="N11" s="147">
         <v>0.2146527</v>
       </c>
-      <c r="O11" s="178">
+      <c r="O11" s="147">
         <v>0.12717339999999999</v>
       </c>
       <c r="P11" s="41">
         <f t="shared" si="4"/>
         <v>1.6878741938172606</v>
       </c>
-      <c r="Q11" s="178">
+      <c r="Q11" s="147">
         <v>0.2160773</v>
       </c>
-      <c r="R11" s="178">
+      <c r="R11" s="147">
         <v>0.1282836</v>
       </c>
       <c r="S11" s="42">
@@ -19068,10 +18998,10 @@
         <f t="shared" si="6"/>
         <v>7.9127593931771729</v>
       </c>
-      <c r="W11" s="178">
+      <c r="W11" s="147">
         <v>0.40067540000000001</v>
       </c>
-      <c r="X11" s="178">
+      <c r="X11" s="147">
         <v>5.6422E-2</v>
       </c>
       <c r="Y11" s="42">
@@ -19083,60 +19013,60 @@
       <c r="A12" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="178">
+      <c r="B12" s="147">
         <v>0.1434242</v>
       </c>
-      <c r="C12" s="178">
+      <c r="C12" s="147">
         <v>3.7123499999999997E-2</v>
       </c>
       <c r="D12" s="35">
         <f t="shared" si="0"/>
         <v>3.8634342128301484</v>
       </c>
-      <c r="E12" s="178">
+      <c r="E12" s="147">
         <v>0.1421936</v>
       </c>
-      <c r="F12" s="178">
+      <c r="F12" s="147">
         <v>4.0946900000000001E-2</v>
       </c>
       <c r="G12" s="36">
         <f t="shared" si="1"/>
         <v>3.4726340699784353</v>
       </c>
-      <c r="H12" s="178">
+      <c r="H12" s="147">
         <v>9.3588099999999994E-2</v>
       </c>
-      <c r="I12" s="178">
+      <c r="I12" s="147">
         <v>2.0167899999999999E-2</v>
       </c>
       <c r="J12" s="36">
         <f t="shared" si="2"/>
         <v>4.6404484353849433</v>
       </c>
-      <c r="K12" s="178">
+      <c r="K12" s="147">
         <v>9.12385E-2</v>
       </c>
-      <c r="L12" s="178">
+      <c r="L12" s="147">
         <v>2.13613E-2</v>
       </c>
       <c r="M12" s="35">
         <f t="shared" si="3"/>
         <v>4.2712054041654772</v>
       </c>
-      <c r="N12" s="178">
+      <c r="N12" s="147">
         <v>9.0120500000000006E-2</v>
       </c>
-      <c r="O12" s="178">
+      <c r="O12" s="147">
         <v>4.1924500000000003E-2</v>
       </c>
       <c r="P12" s="35">
         <f t="shared" si="4"/>
         <v>2.1495903350069767</v>
       </c>
-      <c r="Q12" s="178">
+      <c r="Q12" s="147">
         <v>8.9516999999999999E-2</v>
       </c>
-      <c r="R12" s="178">
+      <c r="R12" s="147">
         <v>4.2317E-2</v>
       </c>
       <c r="S12" s="36">
@@ -19153,10 +19083,10 @@
         <f t="shared" si="6"/>
         <v>6.3757976229151456</v>
       </c>
-      <c r="W12" s="178">
+      <c r="W12" s="147">
         <v>9.8446400000000003E-2</v>
       </c>
-      <c r="X12" s="178">
+      <c r="X12" s="147">
         <v>1.8441699999999998E-2</v>
       </c>
       <c r="Y12" s="36">
@@ -19168,60 +19098,60 @@
       <c r="A13" s="13" t="s">
         <v>454</v>
       </c>
-      <c r="B13" s="178">
+      <c r="B13" s="147">
         <v>-0.23550389999999999</v>
       </c>
-      <c r="C13" s="178">
+      <c r="C13" s="147">
         <v>0.1930182</v>
       </c>
       <c r="D13" s="39">
         <f t="shared" si="0"/>
         <v>-1.2201124039080251</v>
       </c>
-      <c r="E13" s="178">
+      <c r="E13" s="147">
         <v>-0.23141020000000001</v>
       </c>
-      <c r="F13" s="178">
+      <c r="F13" s="147">
         <v>0.2082079</v>
       </c>
       <c r="G13" s="40">
         <f t="shared" si="1"/>
         <v>-1.1114381346721234</v>
       </c>
-      <c r="H13" s="178">
+      <c r="H13" s="147">
         <v>-0.21154909999999999</v>
       </c>
-      <c r="I13" s="178">
+      <c r="I13" s="147">
         <v>9.5172800000000002E-2</v>
       </c>
       <c r="J13" s="40">
         <f t="shared" si="2"/>
         <v>-2.2227894944774134</v>
       </c>
-      <c r="K13" s="178">
+      <c r="K13" s="147">
         <v>-0.20703460000000001</v>
       </c>
-      <c r="L13" s="178">
+      <c r="L13" s="147">
         <v>9.99443E-2</v>
       </c>
       <c r="M13" s="39">
         <f t="shared" si="3"/>
         <v>-2.0714998254027495</v>
       </c>
-      <c r="N13" s="178">
+      <c r="N13" s="147">
         <v>-0.2450801</v>
       </c>
-      <c r="O13" s="178">
+      <c r="O13" s="147">
         <v>0.19110469999999999</v>
       </c>
       <c r="P13" s="39">
         <f t="shared" si="4"/>
         <v>-1.2824388934442743</v>
       </c>
-      <c r="Q13" s="178">
+      <c r="Q13" s="147">
         <v>-0.24443319999999999</v>
       </c>
-      <c r="R13" s="178">
+      <c r="R13" s="147">
         <v>0.1925306</v>
       </c>
       <c r="S13" s="40">
@@ -19238,10 +19168,10 @@
         <f t="shared" si="6"/>
         <v>-2.7866112992777494</v>
       </c>
-      <c r="W13" s="178">
+      <c r="W13" s="147">
         <v>-0.1996484</v>
       </c>
-      <c r="X13" s="178">
+      <c r="X13" s="147">
         <v>8.6045999999999997E-2</v>
       </c>
       <c r="Y13" s="40">
@@ -19250,63 +19180,63 @@
       </c>
     </row>
     <row r="14" spans="1:25" ht="19" thickBot="1">
-      <c r="A14" s="180" t="s">
+      <c r="A14" s="149" t="s">
         <v>470</v>
       </c>
-      <c r="B14" s="178">
+      <c r="B14" s="147">
         <v>0.53330010000000005</v>
       </c>
-      <c r="C14" s="178">
+      <c r="C14" s="147">
         <v>0.1785505</v>
       </c>
       <c r="D14" s="39">
         <f t="shared" si="0"/>
         <v>2.9868306165482599</v>
       </c>
-      <c r="E14" s="178">
+      <c r="E14" s="147">
         <v>0.53573130000000002</v>
       </c>
-      <c r="F14" s="178">
+      <c r="F14" s="147">
         <v>0.19234789999999999</v>
       </c>
       <c r="G14" s="40">
         <f t="shared" si="1"/>
         <v>2.7852204261133084</v>
       </c>
-      <c r="H14" s="178">
+      <c r="H14" s="147">
         <v>7.6216999999999993E-2</v>
       </c>
-      <c r="I14" s="178">
+      <c r="I14" s="147">
         <v>6.4303899999999997E-2</v>
       </c>
       <c r="J14" s="40">
         <f t="shared" si="2"/>
         <v>1.1852624801917147</v>
       </c>
-      <c r="K14" s="178">
+      <c r="K14" s="147">
         <v>7.3127300000000006E-2</v>
       </c>
-      <c r="L14" s="178">
+      <c r="L14" s="147">
         <v>6.7308699999999999E-2</v>
       </c>
       <c r="M14" s="39">
         <f t="shared" si="3"/>
         <v>1.0864464772013129</v>
       </c>
-      <c r="N14" s="178">
+      <c r="N14" s="147">
         <v>-0.116635</v>
       </c>
-      <c r="O14" s="178">
+      <c r="O14" s="147">
         <v>0.12718499999999999</v>
       </c>
       <c r="P14" s="39">
         <f t="shared" si="4"/>
         <v>-0.91704996658410987</v>
       </c>
-      <c r="Q14" s="178">
+      <c r="Q14" s="147">
         <v>-0.1157933</v>
       </c>
-      <c r="R14" s="178">
+      <c r="R14" s="147">
         <v>0.1283958</v>
       </c>
       <c r="S14" s="40">
@@ -19323,10 +19253,10 @@
         <f t="shared" si="6"/>
         <v>1.8790973408415168</v>
       </c>
-      <c r="W14" s="178">
+      <c r="W14" s="147">
         <v>9.8151000000000002E-2</v>
       </c>
-      <c r="X14" s="178">
+      <c r="X14" s="147">
         <v>6.10314E-2</v>
       </c>
       <c r="Y14" s="40">
@@ -19338,60 +19268,60 @@
       <c r="A15" s="15" t="s">
         <v>469</v>
       </c>
-      <c r="B15" s="178">
+      <c r="B15" s="147">
         <v>-0.1162036</v>
       </c>
-      <c r="C15" s="178">
+      <c r="C15" s="147">
         <v>7.2152499999999994E-2</v>
       </c>
       <c r="D15" s="41">
         <f t="shared" si="0"/>
         <v>-1.6105277017428365</v>
       </c>
-      <c r="E15" s="178">
+      <c r="E15" s="147">
         <v>-0.1093326</v>
       </c>
-      <c r="F15" s="178">
+      <c r="F15" s="147">
         <v>7.8919900000000001E-2</v>
       </c>
       <c r="G15" s="42">
         <f t="shared" si="1"/>
         <v>-1.3853616134840516</v>
       </c>
-      <c r="H15" s="178">
+      <c r="H15" s="147">
         <v>-5.8997300000000003E-2</v>
       </c>
-      <c r="I15" s="178">
+      <c r="I15" s="147">
         <v>3.8888199999999998E-2</v>
       </c>
       <c r="J15" s="42">
         <f t="shared" si="2"/>
         <v>-1.5171003029196519</v>
       </c>
-      <c r="K15" s="178">
+      <c r="K15" s="147">
         <v>-5.9267899999999998E-2</v>
       </c>
-      <c r="L15" s="178">
+      <c r="L15" s="147">
         <v>4.1051700000000003E-2</v>
       </c>
       <c r="M15" s="41">
         <f t="shared" si="3"/>
         <v>-1.4437380181575914</v>
       </c>
-      <c r="N15" s="178">
+      <c r="N15" s="147">
         <v>-6.4864500000000005E-2</v>
       </c>
-      <c r="O15" s="178">
+      <c r="O15" s="147">
         <v>8.0999600000000005E-2</v>
       </c>
       <c r="P15" s="41">
         <f t="shared" si="4"/>
         <v>-0.80080025086543638</v>
       </c>
-      <c r="Q15" s="178">
+      <c r="Q15" s="147">
         <v>-6.4970200000000006E-2</v>
       </c>
-      <c r="R15" s="178">
+      <c r="R15" s="147">
         <v>8.1692799999999996E-2</v>
       </c>
       <c r="S15" s="42">
@@ -19408,10 +19338,10 @@
         <f t="shared" si="6"/>
         <v>-2.2401075449931511</v>
       </c>
-      <c r="W15" s="178">
+      <c r="W15" s="147">
         <v>-6.9065699999999994E-2</v>
       </c>
-      <c r="X15" s="178">
+      <c r="X15" s="147">
         <v>3.5372300000000002E-2</v>
       </c>
       <c r="Y15" s="42">
@@ -19423,60 +19353,60 @@
       <c r="A16" s="13" t="s">
         <v>460</v>
       </c>
-      <c r="B16" s="178">
+      <c r="B16" s="147">
         <v>1.1235539999999999</v>
       </c>
-      <c r="C16" s="178">
+      <c r="C16" s="147">
         <v>0.28912409999999999</v>
       </c>
       <c r="D16" s="35">
         <f t="shared" si="0"/>
         <v>3.8860613833298574</v>
       </c>
-      <c r="E16" s="178">
+      <c r="E16" s="147">
         <v>1.062403</v>
       </c>
-      <c r="F16" s="178">
+      <c r="F16" s="147">
         <v>0.31442930000000002</v>
       </c>
       <c r="G16" s="36">
         <f t="shared" si="1"/>
         <v>3.3788295174781737</v>
       </c>
-      <c r="H16" s="178">
+      <c r="H16" s="147">
         <v>0.4857843</v>
       </c>
-      <c r="I16" s="178">
+      <c r="I16" s="147">
         <v>0.15635840000000001</v>
       </c>
       <c r="J16" s="36">
         <f t="shared" si="2"/>
         <v>3.1068641019606238</v>
       </c>
-      <c r="K16" s="178">
+      <c r="K16" s="147">
         <v>0.46754960000000001</v>
       </c>
-      <c r="L16" s="178">
+      <c r="L16" s="147">
         <v>0.1646262</v>
       </c>
       <c r="M16" s="35">
         <f t="shared" si="3"/>
         <v>2.8400679843184133</v>
       </c>
-      <c r="N16" s="178">
+      <c r="N16" s="147">
         <v>0.19195770000000001</v>
       </c>
-      <c r="O16" s="178">
+      <c r="O16" s="147">
         <v>0.3283816</v>
       </c>
       <c r="P16" s="35">
         <f t="shared" si="4"/>
         <v>0.58455680829863799</v>
       </c>
-      <c r="Q16" s="178">
+      <c r="Q16" s="147">
         <v>0.18362139999999999</v>
       </c>
-      <c r="R16" s="178">
+      <c r="R16" s="147">
         <v>0.33264110000000002</v>
       </c>
       <c r="S16" s="36">
@@ -19493,10 +19423,10 @@
         <f t="shared" si="6"/>
         <v>4.6140302896982526</v>
       </c>
-      <c r="W16" s="178">
+      <c r="W16" s="147">
         <v>0.53833839999999999</v>
       </c>
-      <c r="X16" s="178">
+      <c r="X16" s="147">
         <v>0.14080319999999999</v>
       </c>
       <c r="Y16" s="36">
@@ -19508,60 +19438,60 @@
       <c r="A17" s="13" t="s">
         <v>461</v>
       </c>
-      <c r="B17" s="178">
+      <c r="B17" s="147">
         <v>-0.48650450000000001</v>
       </c>
-      <c r="C17" s="178">
+      <c r="C17" s="147">
         <v>0.21072840000000001</v>
       </c>
       <c r="D17" s="35">
         <f t="shared" si="0"/>
         <v>-2.3086802728061335</v>
       </c>
-      <c r="E17" s="178">
+      <c r="E17" s="147">
         <v>-0.43390669999999998</v>
       </c>
-      <c r="F17" s="178">
+      <c r="F17" s="147">
         <v>0.230161</v>
       </c>
       <c r="G17" s="36">
         <f t="shared" si="1"/>
         <v>-1.8852312077198135</v>
       </c>
-      <c r="H17" s="178">
+      <c r="H17" s="147">
         <v>-0.1087288</v>
       </c>
-      <c r="I17" s="178">
+      <c r="I17" s="147">
         <v>0.1087186</v>
       </c>
       <c r="J17" s="40">
         <f t="shared" si="2"/>
         <v>-1.000093820192681</v>
       </c>
-      <c r="K17" s="178">
+      <c r="K17" s="147">
         <v>-0.10343769999999999</v>
       </c>
-      <c r="L17" s="178">
+      <c r="L17" s="147">
         <v>0.1138994</v>
       </c>
       <c r="M17" s="39">
         <f t="shared" si="3"/>
         <v>-0.90814964784713526</v>
       </c>
-      <c r="N17" s="178">
+      <c r="N17" s="147">
         <v>-0.2134316</v>
       </c>
-      <c r="O17" s="178">
+      <c r="O17" s="147">
         <v>0.2257556</v>
       </c>
       <c r="P17" s="39">
         <f t="shared" si="4"/>
         <v>-0.94540999204449416</v>
       </c>
-      <c r="Q17" s="178">
+      <c r="Q17" s="147">
         <v>-0.2106179</v>
       </c>
-      <c r="R17" s="178">
+      <c r="R17" s="147">
         <v>0.22754779999999999</v>
       </c>
       <c r="S17" s="40">
@@ -19578,10 +19508,10 @@
         <f t="shared" si="6"/>
         <v>-2.1667204087707113</v>
       </c>
-      <c r="W17" s="178">
+      <c r="W17" s="147">
         <v>-0.17557539999999999</v>
       </c>
-      <c r="X17" s="178">
+      <c r="X17" s="147">
         <v>9.8251699999999997E-2</v>
       </c>
       <c r="Y17" s="40">
@@ -19593,60 +19523,60 @@
       <c r="A18" s="13" t="s">
         <v>473</v>
       </c>
-      <c r="B18" s="178">
+      <c r="B18" s="147">
         <v>-1.14313E-2</v>
       </c>
-      <c r="C18" s="178">
+      <c r="C18" s="147">
         <v>0.108363</v>
       </c>
       <c r="D18" s="39">
         <f t="shared" ref="D18:D23" si="8">B18/C18</f>
         <v>-0.10549080405673524</v>
       </c>
-      <c r="E18" s="178">
+      <c r="E18" s="147">
         <v>-1.90145E-2</v>
       </c>
-      <c r="F18" s="178">
+      <c r="F18" s="147">
         <v>0.11713800000000001</v>
       </c>
       <c r="G18" s="39">
         <f t="shared" si="1"/>
         <v>-0.16232563301405178</v>
       </c>
-      <c r="H18" s="178">
+      <c r="H18" s="147">
         <v>2.5736000000000001E-3</v>
       </c>
-      <c r="I18" s="178">
+      <c r="I18" s="147">
         <v>5.77977E-2</v>
       </c>
       <c r="J18" s="39">
         <f t="shared" si="2"/>
         <v>4.4527723421520234E-2</v>
       </c>
-      <c r="K18" s="178">
+      <c r="K18" s="147">
         <v>-1.1942000000000001E-3</v>
       </c>
-      <c r="L18" s="178">
+      <c r="L18" s="147">
         <v>6.0827600000000003E-2</v>
       </c>
       <c r="M18" s="39">
         <f t="shared" si="3"/>
         <v>-1.9632535230717636E-2</v>
       </c>
-      <c r="N18" s="178">
+      <c r="N18" s="147">
         <v>0.32590439999999998</v>
       </c>
-      <c r="O18" s="178">
+      <c r="O18" s="147">
         <v>0.1240695</v>
       </c>
       <c r="P18" s="39">
         <f t="shared" si="4"/>
         <v>2.626789017445867</v>
       </c>
-      <c r="Q18" s="178">
+      <c r="Q18" s="147">
         <v>0.32606350000000001</v>
       </c>
-      <c r="R18" s="178">
+      <c r="R18" s="147">
         <v>0.12507070000000001</v>
       </c>
       <c r="S18" s="39">
@@ -19663,10 +19593,10 @@
         <f t="shared" si="6"/>
         <v>1.098238621999486</v>
       </c>
-      <c r="W18" s="178">
+      <c r="W18" s="147">
         <v>4.37858E-2</v>
       </c>
-      <c r="X18" s="178">
+      <c r="X18" s="147">
         <v>5.2449299999999997E-2</v>
       </c>
       <c r="Y18" s="39">
@@ -19678,60 +19608,60 @@
       <c r="A19" s="13" t="s">
         <v>479</v>
       </c>
-      <c r="B19" s="178">
+      <c r="B19" s="147">
         <v>-0.28524559999999999</v>
       </c>
-      <c r="C19" s="178">
+      <c r="C19" s="147">
         <v>0.15450050000000001</v>
       </c>
       <c r="D19" s="39">
         <f t="shared" si="8"/>
         <v>-1.8462438632884681</v>
       </c>
-      <c r="E19" s="178">
+      <c r="E19" s="147">
         <v>-0.29631099999999999</v>
       </c>
-      <c r="F19" s="178">
+      <c r="F19" s="147">
         <v>0.16617750000000001</v>
       </c>
       <c r="G19" s="39">
         <f t="shared" si="1"/>
         <v>-1.7830993967294007</v>
       </c>
-      <c r="H19" s="178">
+      <c r="H19" s="147">
         <v>-0.1243765</v>
       </c>
-      <c r="I19" s="178">
+      <c r="I19" s="147">
         <v>7.6474100000000003E-2</v>
       </c>
       <c r="J19" s="39">
         <f t="shared" si="2"/>
         <v>-1.6263872343708523</v>
       </c>
-      <c r="K19" s="178">
+      <c r="K19" s="147">
         <v>-0.1205672</v>
       </c>
-      <c r="L19" s="178">
+      <c r="L19" s="147">
         <v>8.0062900000000006E-2</v>
       </c>
       <c r="M19" s="39">
         <f t="shared" si="3"/>
         <v>-1.5059059814221067</v>
       </c>
-      <c r="N19" s="178">
+      <c r="N19" s="147">
         <v>-0.1194987</v>
       </c>
-      <c r="O19" s="178">
+      <c r="O19" s="147">
         <v>0.1518265</v>
       </c>
       <c r="P19" s="39">
         <f t="shared" si="4"/>
         <v>-0.78707406151100101</v>
       </c>
-      <c r="Q19" s="178">
+      <c r="Q19" s="147">
         <v>-0.1173409</v>
       </c>
-      <c r="R19" s="178">
+      <c r="R19" s="147">
         <v>0.15329329999999999</v>
       </c>
       <c r="S19" s="39">
@@ -19748,10 +19678,10 @@
         <f t="shared" si="6"/>
         <v>-2.4083454468817562</v>
       </c>
-      <c r="W19" s="178">
+      <c r="W19" s="147">
         <v>-0.14009869999999999</v>
       </c>
-      <c r="X19" s="178">
+      <c r="X19" s="147">
         <v>6.8941799999999998E-2</v>
       </c>
       <c r="Y19" s="39">
@@ -19763,60 +19693,60 @@
       <c r="A20" s="13" t="s">
         <v>462</v>
       </c>
-      <c r="B20" s="178">
+      <c r="B20" s="147">
         <v>0.2060834</v>
       </c>
-      <c r="C20" s="178">
+      <c r="C20" s="147">
         <v>0.11580849999999999</v>
       </c>
       <c r="D20" s="39">
         <f t="shared" si="8"/>
         <v>1.77951877452864</v>
       </c>
-      <c r="E20" s="178">
+      <c r="E20" s="147">
         <v>0.19420370000000001</v>
       </c>
-      <c r="F20" s="178">
+      <c r="F20" s="147">
         <v>0.12851180000000001</v>
       </c>
       <c r="G20" s="39">
         <f t="shared" si="1"/>
         <v>1.511174071174787</v>
       </c>
-      <c r="H20" s="178">
+      <c r="H20" s="147">
         <v>0.1191953</v>
       </c>
-      <c r="I20" s="178">
+      <c r="I20" s="147">
         <v>6.5876500000000004E-2</v>
       </c>
       <c r="J20" s="39">
         <f t="shared" si="2"/>
         <v>1.8093751185931251</v>
       </c>
-      <c r="K20" s="178">
+      <c r="K20" s="147">
         <v>0.1214098</v>
       </c>
-      <c r="L20" s="178">
+      <c r="L20" s="147">
         <v>6.9661799999999996E-2</v>
       </c>
       <c r="M20" s="39">
         <f t="shared" si="3"/>
         <v>1.7428461509751401</v>
       </c>
-      <c r="N20" s="178">
+      <c r="N20" s="147">
         <v>-5.85858E-2</v>
       </c>
-      <c r="O20" s="178">
+      <c r="O20" s="147">
         <v>0.1704542</v>
       </c>
       <c r="P20" s="39">
         <f t="shared" si="4"/>
         <v>-0.34370405657355468</v>
       </c>
-      <c r="Q20" s="178">
+      <c r="Q20" s="147">
         <v>-5.9255799999999997E-2</v>
       </c>
-      <c r="R20" s="178">
+      <c r="R20" s="147">
         <v>0.1720516</v>
       </c>
       <c r="S20" s="39">
@@ -19833,10 +19763,10 @@
         <f t="shared" si="6"/>
         <v>2.2039724811772063</v>
       </c>
-      <c r="W20" s="178">
+      <c r="W20" s="147">
         <v>0.1191682</v>
       </c>
-      <c r="X20" s="178">
+      <c r="X20" s="147">
         <v>6.1495000000000001E-2</v>
       </c>
       <c r="Y20" s="39">
@@ -19848,60 +19778,60 @@
       <c r="A21" s="13" t="s">
         <v>463</v>
       </c>
-      <c r="B21" s="178">
+      <c r="B21" s="147">
         <v>-0.15743090000000001</v>
       </c>
-      <c r="C21" s="178">
+      <c r="C21" s="147">
         <v>0.17751220000000001</v>
       </c>
       <c r="D21" s="39">
         <f t="shared" si="8"/>
         <v>-0.88687369093504564</v>
       </c>
-      <c r="E21" s="178">
+      <c r="E21" s="147">
         <v>-0.15635979999999999</v>
       </c>
-      <c r="F21" s="178">
+      <c r="F21" s="147">
         <v>0.19192819999999999</v>
       </c>
       <c r="G21" s="39">
         <f t="shared" si="1"/>
         <v>-0.81467861419009813</v>
       </c>
-      <c r="H21" s="178">
+      <c r="H21" s="147">
         <v>-0.24706710000000001</v>
       </c>
-      <c r="I21" s="178">
+      <c r="I21" s="147">
         <v>9.2806200000000005E-2</v>
       </c>
       <c r="J21" s="39">
         <f t="shared" si="2"/>
         <v>-2.6621831300064005</v>
       </c>
-      <c r="K21" s="178">
+      <c r="K21" s="147">
         <v>-0.24111479999999999</v>
       </c>
-      <c r="L21" s="178">
+      <c r="L21" s="147">
         <v>9.7394800000000004E-2</v>
       </c>
       <c r="M21" s="39">
         <f t="shared" si="3"/>
         <v>-2.4756434635113989</v>
       </c>
-      <c r="N21" s="178">
+      <c r="N21" s="147">
         <v>-2.54314E-2</v>
       </c>
-      <c r="O21" s="178">
+      <c r="O21" s="147">
         <v>0.19763149999999999</v>
       </c>
       <c r="P21" s="39">
         <f t="shared" si="4"/>
         <v>-0.1286809036008936</v>
       </c>
-      <c r="Q21" s="178">
+      <c r="Q21" s="147">
         <v>-2.2649499999999999E-2</v>
       </c>
-      <c r="R21" s="178">
+      <c r="R21" s="147">
         <v>0.1992932</v>
       </c>
       <c r="S21" s="39">
@@ -19918,10 +19848,10 @@
         <f t="shared" si="6"/>
         <v>-2.5886728593570432</v>
       </c>
-      <c r="W21" s="178">
+      <c r="W21" s="147">
         <v>-0.1811507</v>
       </c>
-      <c r="X21" s="178">
+      <c r="X21" s="147">
         <v>8.4043800000000002E-2</v>
       </c>
       <c r="Y21" s="39">
@@ -19933,60 +19863,60 @@
       <c r="A22" s="13" t="s">
         <v>474</v>
       </c>
-      <c r="B22" s="178">
+      <c r="B22" s="147">
         <v>0.1097588</v>
       </c>
-      <c r="C22" s="178">
+      <c r="C22" s="147">
         <v>0.13677300000000001</v>
       </c>
       <c r="D22" s="39">
         <f t="shared" si="8"/>
         <v>0.80248879530316652</v>
       </c>
-      <c r="E22" s="178">
+      <c r="E22" s="147">
         <v>0.1012227</v>
       </c>
-      <c r="F22" s="178">
+      <c r="F22" s="147">
         <v>0.14764050000000001</v>
       </c>
       <c r="G22" s="39">
         <f t="shared" si="1"/>
         <v>0.68560252776169139</v>
       </c>
-      <c r="H22" s="178">
+      <c r="H22" s="147">
         <v>0.15877810000000001</v>
       </c>
-      <c r="I22" s="178">
+      <c r="I22" s="147">
         <v>7.5855699999999998E-2</v>
       </c>
       <c r="J22" s="39">
         <f t="shared" si="2"/>
         <v>2.0931597757320808</v>
       </c>
-      <c r="K22" s="178">
+      <c r="K22" s="147">
         <v>0.16272900000000001</v>
       </c>
-      <c r="L22" s="178">
+      <c r="L22" s="147">
         <v>7.9640600000000006E-2</v>
       </c>
       <c r="M22" s="39">
         <f t="shared" si="3"/>
         <v>2.0432919892617583</v>
       </c>
-      <c r="N22" s="178">
+      <c r="N22" s="147">
         <v>0.13555030000000001</v>
       </c>
-      <c r="O22" s="178">
+      <c r="O22" s="147">
         <v>0.15733169999999999</v>
       </c>
       <c r="P22" s="39">
         <f t="shared" si="4"/>
         <v>0.86155746108381226</v>
       </c>
-      <c r="Q22" s="178">
+      <c r="Q22" s="147">
         <v>0.1366665</v>
       </c>
-      <c r="R22" s="178">
+      <c r="R22" s="147">
         <v>0.15862680000000001</v>
       </c>
       <c r="S22" s="39">
@@ -20003,10 +19933,10 @@
         <f t="shared" si="6"/>
         <v>2.4595379747768766</v>
       </c>
-      <c r="W22" s="178">
+      <c r="W22" s="147">
         <v>0.15410950000000001</v>
       </c>
-      <c r="X22" s="178">
+      <c r="X22" s="147">
         <v>6.7916199999999996E-2</v>
       </c>
       <c r="Y22" s="39">
@@ -20015,63 +19945,63 @@
       </c>
     </row>
     <row r="23" spans="1:25" ht="19" thickBot="1">
-      <c r="A23" s="180" t="s">
+      <c r="A23" s="149" t="s">
         <v>467</v>
       </c>
-      <c r="B23" s="178">
+      <c r="B23" s="147">
         <v>-8.7895399999999999E-2</v>
       </c>
-      <c r="C23" s="178">
+      <c r="C23" s="147">
         <v>0.1426539</v>
       </c>
       <c r="D23" s="39">
         <f t="shared" si="8"/>
         <v>-0.61614438862169207</v>
       </c>
-      <c r="E23" s="178">
+      <c r="E23" s="147">
         <v>-0.1107496</v>
       </c>
-      <c r="F23" s="178">
+      <c r="F23" s="147">
         <v>0.1532046</v>
       </c>
       <c r="G23" s="39">
         <f t="shared" si="1"/>
         <v>-0.72288691070633648</v>
       </c>
-      <c r="H23" s="178">
+      <c r="H23" s="147">
         <v>0.1194219</v>
       </c>
-      <c r="I23" s="178">
+      <c r="I23" s="147">
         <v>7.4553300000000003E-2</v>
       </c>
       <c r="J23" s="39">
         <f t="shared" si="2"/>
         <v>1.6018325144561005</v>
       </c>
-      <c r="K23" s="178">
+      <c r="K23" s="147">
         <v>0.1175929</v>
       </c>
-      <c r="L23" s="178">
+      <c r="L23" s="147">
         <v>7.8412800000000005E-2</v>
       </c>
       <c r="M23" s="39">
         <f t="shared" si="3"/>
         <v>1.4996645955762324</v>
       </c>
-      <c r="N23" s="178">
+      <c r="N23" s="147">
         <v>0.32137979999999999</v>
       </c>
-      <c r="O23" s="178">
+      <c r="O23" s="147">
         <v>0.1542617</v>
       </c>
       <c r="P23" s="39">
         <f t="shared" si="4"/>
         <v>2.0833414904671734</v>
       </c>
-      <c r="Q23" s="178">
+      <c r="Q23" s="147">
         <v>0.3208008</v>
       </c>
-      <c r="R23" s="178">
+      <c r="R23" s="147">
         <v>0.15533739999999999</v>
       </c>
       <c r="S23" s="39">
@@ -20088,10 +20018,10 @@
         <f t="shared" si="6"/>
         <v>1.943787884030177</v>
       </c>
-      <c r="W23" s="178">
+      <c r="W23" s="147">
         <v>0.1102788</v>
       </c>
-      <c r="X23" s="178">
+      <c r="X23" s="147">
         <v>6.7479700000000004E-2</v>
       </c>
       <c r="Y23" s="39">
@@ -20100,66 +20030,66 @@
       </c>
     </row>
     <row r="24" spans="1:25" ht="19" thickBot="1">
-      <c r="A24" s="180" t="s">
+      <c r="A24" s="149" t="s">
         <v>481</v>
       </c>
-      <c r="B24" s="207">
+      <c r="B24" s="176">
         <v>-5.5004</v>
       </c>
-      <c r="C24" s="202">
+      <c r="C24" s="171">
         <v>0.69567650000000003</v>
       </c>
-      <c r="D24" s="206">
+      <c r="D24" s="175">
         <f t="shared" ref="D24" si="9">B24/C24</f>
         <v>-7.9065485178815154</v>
       </c>
-      <c r="E24" s="202">
+      <c r="E24" s="171">
         <v>-5.3812530000000001</v>
       </c>
-      <c r="F24" s="202">
+      <c r="F24" s="171">
         <v>0.75940300000000005</v>
       </c>
-      <c r="G24" s="206">
+      <c r="G24" s="175">
         <f t="shared" ref="G24" si="10">E24/F24</f>
         <v>-7.0861624196902033</v>
       </c>
-      <c r="H24" s="202">
+      <c r="H24" s="171">
         <v>-1.8091280000000001</v>
       </c>
-      <c r="I24" s="202">
+      <c r="I24" s="171">
         <v>0.35283540000000002</v>
       </c>
-      <c r="J24" s="206">
+      <c r="J24" s="175">
         <f t="shared" ref="J24" si="11">H24/I24</f>
         <v>-5.1273993482513376</v>
       </c>
-      <c r="K24" s="202">
+      <c r="K24" s="171">
         <v>-1.7421139999999999</v>
       </c>
-      <c r="L24" s="202">
+      <c r="L24" s="171">
         <v>0.37458989999999998</v>
       </c>
-      <c r="M24" s="206">
+      <c r="M24" s="175">
         <f t="shared" ref="M24" si="12">K24/L24</f>
         <v>-4.6507233644046462</v>
       </c>
-      <c r="N24" s="202">
+      <c r="N24" s="171">
         <v>-2.2656000000000001</v>
       </c>
-      <c r="O24" s="202">
+      <c r="O24" s="171">
         <v>0.73780829999999997</v>
       </c>
-      <c r="P24" s="206">
+      <c r="P24" s="175">
         <f t="shared" ref="P24" si="13">N24/O24</f>
         <v>-3.0707163364792724</v>
       </c>
-      <c r="Q24" s="202">
+      <c r="Q24" s="171">
         <v>-2.2513969999999999</v>
       </c>
-      <c r="R24" s="202">
+      <c r="R24" s="171">
         <v>0.74664450000000004</v>
       </c>
-      <c r="S24" s="206">
+      <c r="S24" s="175">
         <f t="shared" ref="S24" si="14">Q24/R24</f>
         <v>-3.0153533575885172</v>
       </c>
@@ -20169,74 +20099,74 @@
       <c r="U24" s="14">
         <v>0.28662840000000001</v>
       </c>
-      <c r="V24" s="206">
+      <c r="V24" s="175">
         <f t="shared" ref="V24" si="15">T24/U24</f>
         <v>-5.7089702206759689</v>
       </c>
-      <c r="W24" s="202">
+      <c r="W24" s="171">
         <v>-1.498389</v>
       </c>
-      <c r="X24" s="202">
+      <c r="X24" s="171">
         <v>0.32390649999999999</v>
       </c>
-      <c r="Y24" s="193">
+      <c r="Y24" s="162">
         <f t="shared" ref="Y24" si="16">W24/X24</f>
         <v>-4.625992377429907</v>
       </c>
     </row>
     <row r="25" spans="1:25" ht="20" thickBot="1">
-      <c r="A25" s="189" t="s">
+      <c r="A25" s="158" t="s">
         <v>484</v>
       </c>
-      <c r="B25" s="203"/>
-      <c r="C25" s="204"/>
-      <c r="D25" s="204"/>
-      <c r="E25" s="202">
+      <c r="B25" s="172"/>
+      <c r="C25" s="173"/>
+      <c r="D25" s="173"/>
+      <c r="E25" s="171">
         <v>-1.6472910000000001</v>
       </c>
-      <c r="F25" s="202">
+      <c r="F25" s="171">
         <v>0.49839349999999999</v>
       </c>
-      <c r="G25" s="193">
+      <c r="G25" s="162">
         <f>E25/F25</f>
         <v>-3.3052016127818682</v>
       </c>
-      <c r="H25" s="203"/>
-      <c r="I25" s="204"/>
-      <c r="J25" s="205"/>
-      <c r="K25" s="202">
+      <c r="H25" s="172"/>
+      <c r="I25" s="173"/>
+      <c r="J25" s="174"/>
+      <c r="K25" s="171">
         <v>-2.2025779999999999</v>
       </c>
-      <c r="L25" s="202">
+      <c r="L25" s="171">
         <v>0.6728073</v>
       </c>
-      <c r="M25" s="206">
+      <c r="M25" s="175">
         <f>K25/L25</f>
         <v>-3.2737129933043234</v>
       </c>
-      <c r="N25" s="203"/>
-      <c r="O25" s="204"/>
-      <c r="P25" s="204"/>
-      <c r="Q25" s="202">
+      <c r="N25" s="172"/>
+      <c r="O25" s="173"/>
+      <c r="P25" s="173"/>
+      <c r="Q25" s="171">
         <v>-4.104552</v>
       </c>
-      <c r="R25" s="202">
+      <c r="R25" s="171">
         <v>4.3833780000000004</v>
       </c>
-      <c r="S25" s="193">
+      <c r="S25" s="162">
         <f>Q25/R25</f>
         <v>-0.93639015389500968</v>
       </c>
-      <c r="T25" s="204"/>
-      <c r="U25" s="204"/>
-      <c r="V25" s="204"/>
-      <c r="W25" s="202">
+      <c r="T25" s="173"/>
+      <c r="U25" s="173"/>
+      <c r="V25" s="173"/>
+      <c r="W25" s="171">
         <v>-1.3623130000000001</v>
       </c>
-      <c r="X25" s="202">
+      <c r="X25" s="171">
         <v>0.31210260000000001</v>
       </c>
-      <c r="Y25" s="193">
+      <c r="Y25" s="162">
         <f>W25/X25</f>
         <v>-4.364952422696895</v>
       </c>
@@ -20245,55 +20175,55 @@
       <c r="A26" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="200"/>
-      <c r="C26" s="201"/>
-      <c r="D26" s="201"/>
-      <c r="E26" s="202">
+      <c r="B26" s="169"/>
+      <c r="C26" s="170"/>
+      <c r="D26" s="170"/>
+      <c r="E26" s="171">
         <v>0.19257079999999999</v>
       </c>
-      <c r="F26" s="202">
+      <c r="F26" s="171">
         <v>9.5976000000000006E-2</v>
       </c>
-      <c r="G26" s="193">
+      <c r="G26" s="162">
         <f>E26/F26</f>
         <v>2.0064474451946319</v>
       </c>
-      <c r="H26" s="201"/>
-      <c r="I26" s="201"/>
-      <c r="J26" s="201"/>
-      <c r="K26" s="202">
+      <c r="H26" s="170"/>
+      <c r="I26" s="170"/>
+      <c r="J26" s="170"/>
+      <c r="K26" s="171">
         <v>0.1105179</v>
       </c>
-      <c r="L26" s="202">
+      <c r="L26" s="171">
         <v>7.4357199999999998E-2</v>
       </c>
-      <c r="M26" s="193">
+      <c r="M26" s="162">
         <f>K26/L26</f>
         <v>1.4863106733443434</v>
       </c>
-      <c r="N26" s="201"/>
-      <c r="O26" s="201"/>
-      <c r="P26" s="201"/>
-      <c r="Q26" s="202">
+      <c r="N26" s="170"/>
+      <c r="O26" s="170"/>
+      <c r="P26" s="170"/>
+      <c r="Q26" s="171">
         <v>1.6497399999999999E-2</v>
       </c>
-      <c r="R26" s="202">
+      <c r="R26" s="171">
         <v>7.2314400000000001E-2</v>
       </c>
-      <c r="S26" s="193">
+      <c r="S26" s="162">
         <f>Q26/R26</f>
         <v>0.22813436881174426</v>
       </c>
-      <c r="T26" s="201"/>
-      <c r="U26" s="201"/>
-      <c r="V26" s="201"/>
-      <c r="W26" s="202">
+      <c r="T26" s="170"/>
+      <c r="U26" s="170"/>
+      <c r="V26" s="170"/>
+      <c r="W26" s="171">
         <v>0.25606770000000001</v>
       </c>
-      <c r="X26" s="202">
+      <c r="X26" s="171">
         <v>7.9919400000000002E-2</v>
       </c>
-      <c r="Y26" s="193">
+      <c r="Y26" s="162">
         <f>W26/X26</f>
         <v>3.2040743549125743</v>
       </c>
@@ -20302,11 +20232,11 @@
       <c r="A27" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="208">
+      <c r="B27" s="177">
         <v>434</v>
       </c>
-      <c r="C27" s="191"/>
-      <c r="D27" s="192"/>
+      <c r="C27" s="160"/>
+      <c r="D27" s="161"/>
       <c r="E27" s="10">
         <v>434</v>
       </c>
@@ -20347,7 +20277,7 @@
       <c r="A28" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="209">
+      <c r="B28" s="178">
         <v>-669.29669999999999</v>
       </c>
       <c r="C28" s="50"/>
@@ -20392,7 +20322,7 @@
       <c r="A29" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="209">
+      <c r="B29" s="178">
         <v>-491.9205</v>
       </c>
       <c r="C29" s="50"/>
@@ -20437,7 +20367,7 @@
       <c r="A30" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="209">
+      <c r="B30" s="178">
         <v>20</v>
       </c>
       <c r="C30" s="53"/>
@@ -20482,7 +20412,7 @@
       <c r="A31" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="209">
+      <c r="B31" s="178">
         <v>1023.841</v>
       </c>
       <c r="C31" s="50"/>
@@ -20527,7 +20457,7 @@
       <c r="A32" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="209">
+      <c r="B32" s="178">
         <v>1105.3019999999999</v>
       </c>
       <c r="C32" s="50"/>
@@ -20675,35 +20605,35 @@
       <c r="Y34" s="60"/>
     </row>
     <row r="35" spans="1:25">
-      <c r="B35" s="208"/>
-      <c r="C35" s="187"/>
-      <c r="D35" s="187"/>
-      <c r="E35" s="187"/>
-      <c r="F35" s="187"/>
-      <c r="G35" s="187"/>
-      <c r="H35" s="187"/>
-      <c r="I35" s="187"/>
-      <c r="J35" s="187"/>
-      <c r="K35" s="187"/>
-      <c r="L35" s="187"/>
-      <c r="M35" s="187"/>
-      <c r="N35" s="187"/>
-      <c r="O35" s="187"/>
-      <c r="P35" s="187"/>
-      <c r="Q35" s="187"/>
-      <c r="R35" s="187"/>
-      <c r="S35" s="187"/>
-      <c r="T35" s="212" t="s">
+      <c r="B35" s="177"/>
+      <c r="C35" s="156"/>
+      <c r="D35" s="156"/>
+      <c r="E35" s="156"/>
+      <c r="F35" s="156"/>
+      <c r="G35" s="156"/>
+      <c r="H35" s="156"/>
+      <c r="I35" s="156"/>
+      <c r="J35" s="156"/>
+      <c r="K35" s="156"/>
+      <c r="L35" s="156"/>
+      <c r="M35" s="156"/>
+      <c r="N35" s="156"/>
+      <c r="O35" s="156"/>
+      <c r="P35" s="156"/>
+      <c r="Q35" s="156"/>
+      <c r="R35" s="156"/>
+      <c r="S35" s="156"/>
+      <c r="T35" s="191" t="s">
         <v>504</v>
       </c>
-      <c r="U35" s="210"/>
-      <c r="V35" s="210"/>
-      <c r="W35" s="210"/>
-      <c r="X35" s="210"/>
-      <c r="Y35" s="213"/>
+      <c r="U35" s="192"/>
+      <c r="V35" s="192"/>
+      <c r="W35" s="192"/>
+      <c r="X35" s="192"/>
+      <c r="Y35" s="193"/>
     </row>
     <row r="36" spans="1:25">
-      <c r="B36" s="209"/>
+      <c r="B36" s="178"/>
       <c r="C36" s="20"/>
       <c r="D36" s="20"/>
       <c r="E36" s="20"/>
@@ -20721,18 +20651,18 @@
       <c r="Q36" s="20"/>
       <c r="R36" s="20"/>
       <c r="S36" s="20"/>
-      <c r="T36" s="209"/>
+      <c r="T36" s="178"/>
       <c r="U36" s="20"/>
       <c r="V36" s="20"/>
       <c r="W36" s="20"/>
       <c r="X36" s="20"/>
-      <c r="Y36" s="183"/>
+      <c r="Y36" s="152"/>
     </row>
     <row r="37" spans="1:25" ht="19">
-      <c r="A37" s="211" t="s">
+      <c r="A37" s="179" t="s">
         <v>505</v>
       </c>
-      <c r="B37" s="214">
+      <c r="B37" s="180">
         <f>-2*(B29 - E29)</f>
         <v>5.8032000000000608</v>
       </c>
@@ -20741,7 +20671,7 @@
       <c r="E37" s="20"/>
       <c r="F37" s="20"/>
       <c r="G37" s="20"/>
-      <c r="H37" s="214">
+      <c r="H37" s="180">
         <f>-2*(H29 - K29)</f>
         <v>2.6094000000000506</v>
       </c>
@@ -20750,7 +20680,7 @@
       <c r="K37" s="20"/>
       <c r="L37" s="20"/>
       <c r="M37" s="20"/>
-      <c r="N37" s="214">
+      <c r="N37" s="180">
         <f>-2*(N29 - Q29)</f>
         <v>5.4199999999923421E-2</v>
       </c>
@@ -20759,7 +20689,7 @@
       <c r="Q37" s="20"/>
       <c r="R37" s="20"/>
       <c r="S37" s="20"/>
-      <c r="T37" s="214">
+      <c r="T37" s="180">
         <f>-2*(T29 - W29)</f>
         <v>14.738000000000056</v>
       </c>
@@ -20767,13 +20697,13 @@
       <c r="V37" s="20"/>
       <c r="W37" s="20"/>
       <c r="X37" s="20"/>
-      <c r="Y37" s="183"/>
+      <c r="Y37" s="152"/>
     </row>
     <row r="38" spans="1:25" ht="19">
-      <c r="A38" s="211" t="s">
+      <c r="A38" s="179" t="s">
         <v>506</v>
       </c>
-      <c r="B38" s="215">
+      <c r="B38" s="181">
         <f>(COUNT(E5:E25)-COUNT(B5:B24))</f>
         <v>1</v>
       </c>
@@ -20782,7 +20712,7 @@
       <c r="E38" s="20"/>
       <c r="F38" s="20"/>
       <c r="G38" s="20"/>
-      <c r="H38" s="215">
+      <c r="H38" s="181">
         <f>(COUNT(K5:K25)-COUNT(H5:H24))</f>
         <v>1</v>
       </c>
@@ -20791,7 +20721,7 @@
       <c r="K38" s="20"/>
       <c r="L38" s="20"/>
       <c r="M38" s="20"/>
-      <c r="N38" s="215">
+      <c r="N38" s="181">
         <f>(COUNT(Q5:Q25)-COUNT(N5:N24))</f>
         <v>1</v>
       </c>
@@ -20800,7 +20730,7 @@
       <c r="Q38" s="20"/>
       <c r="R38" s="20"/>
       <c r="S38" s="20"/>
-      <c r="T38" s="215">
+      <c r="T38" s="181">
         <f>(COUNT(W5:W25)-COUNT(T5:T24))</f>
         <v>1</v>
       </c>
@@ -20808,13 +20738,13 @@
       <c r="V38" s="20"/>
       <c r="W38" s="20"/>
       <c r="X38" s="20"/>
-      <c r="Y38" s="183"/>
+      <c r="Y38" s="152"/>
     </row>
     <row r="39" spans="1:25" ht="19">
-      <c r="A39" s="211" t="s">
+      <c r="A39" s="179" t="s">
         <v>507</v>
       </c>
-      <c r="B39" s="214">
+      <c r="B39" s="180">
         <f>1-_xlfn.CHISQ.DIST(B37,B38,TRUE)</f>
         <v>1.5997034867445414E-2</v>
       </c>
@@ -20823,7 +20753,7 @@
       <c r="E39" s="20"/>
       <c r="F39" s="20"/>
       <c r="G39" s="20"/>
-      <c r="H39" s="214">
+      <c r="H39" s="180">
         <f>1-_xlfn.CHISQ.DIST(H37,H38,TRUE)</f>
         <v>0.10623194858647589</v>
       </c>
@@ -20832,7 +20762,7 @@
       <c r="K39" s="20"/>
       <c r="L39" s="20"/>
       <c r="M39" s="20"/>
-      <c r="N39" s="214">
+      <c r="N39" s="180">
         <f>1-_xlfn.CHISQ.DIST(N37,N38,TRUE)</f>
         <v>0.81590977478275717</v>
       </c>
@@ -20841,7 +20771,7 @@
       <c r="Q39" s="20"/>
       <c r="R39" s="20"/>
       <c r="S39" s="20"/>
-      <c r="T39" s="214">
+      <c r="T39" s="180">
         <f>1-_xlfn.CHISQ.DIST(T37,T38,TRUE)</f>
         <v>1.2353125442710056E-4</v>
       </c>
@@ -20849,13 +20779,13 @@
       <c r="V39" s="20"/>
       <c r="W39" s="20"/>
       <c r="X39" s="20"/>
-      <c r="Y39" s="183"/>
+      <c r="Y39" s="152"/>
     </row>
     <row r="40" spans="1:25" ht="19">
-      <c r="A40" s="211" t="s">
+      <c r="A40" s="179" t="s">
         <v>508</v>
       </c>
-      <c r="B40" s="214">
+      <c r="B40" s="180">
         <v>0.01</v>
       </c>
       <c r="C40" s="20"/>
@@ -20863,7 +20793,7 @@
       <c r="E40" s="20"/>
       <c r="F40" s="20"/>
       <c r="G40" s="20"/>
-      <c r="H40" s="214">
+      <c r="H40" s="180">
         <v>0.01</v>
       </c>
       <c r="I40" s="20"/>
@@ -20871,7 +20801,7 @@
       <c r="K40" s="20"/>
       <c r="L40" s="20"/>
       <c r="M40" s="20"/>
-      <c r="N40" s="214">
+      <c r="N40" s="180">
         <v>0.01</v>
       </c>
       <c r="O40" s="20"/>
@@ -20879,20 +20809,20 @@
       <c r="Q40" s="20"/>
       <c r="R40" s="20"/>
       <c r="S40" s="20"/>
-      <c r="T40" s="214">
+      <c r="T40" s="180">
         <v>0.01</v>
       </c>
       <c r="U40" s="20"/>
       <c r="V40" s="20"/>
       <c r="W40" s="20"/>
       <c r="X40" s="20"/>
-      <c r="Y40" s="183"/>
+      <c r="Y40" s="152"/>
     </row>
     <row r="41" spans="1:25" ht="19">
-      <c r="A41" s="211" t="s">
+      <c r="A41" s="179" t="s">
         <v>509</v>
       </c>
-      <c r="B41" s="214">
+      <c r="B41" s="180">
         <f>CHIINV(B40,B38)</f>
         <v>6.6348966010212118</v>
       </c>
@@ -20901,7 +20831,7 @@
       <c r="E41" s="20"/>
       <c r="F41" s="20"/>
       <c r="G41" s="20"/>
-      <c r="H41" s="214">
+      <c r="H41" s="180">
         <f>CHIINV(H40,H38)</f>
         <v>6.6348966010212118</v>
       </c>
@@ -20910,7 +20840,7 @@
       <c r="K41" s="20"/>
       <c r="L41" s="20"/>
       <c r="M41" s="20"/>
-      <c r="N41" s="214">
+      <c r="N41" s="180">
         <f>CHIINV(N40,N38)</f>
         <v>6.6348966010212118</v>
       </c>
@@ -20919,7 +20849,7 @@
       <c r="Q41" s="20"/>
       <c r="R41" s="20"/>
       <c r="S41" s="20"/>
-      <c r="T41" s="214">
+      <c r="T41" s="180">
         <f>CHIINV(T40,T38)</f>
         <v>6.6348966010212118</v>
       </c>
@@ -20927,197 +20857,197 @@
       <c r="V41" s="20"/>
       <c r="W41" s="20"/>
       <c r="X41" s="20"/>
-      <c r="Y41" s="183"/>
+      <c r="Y41" s="152"/>
     </row>
     <row r="42" spans="1:25" ht="20" thickBot="1">
-      <c r="A42" s="211" t="s">
+      <c r="A42" s="179" t="s">
         <v>510</v>
       </c>
-      <c r="B42" s="216" t="str">
+      <c r="B42" s="182" t="str">
         <f>IF(B37&gt;B41,"Accept H1","Accept H0")</f>
         <v>Accept H0</v>
       </c>
-      <c r="C42" s="184"/>
-      <c r="D42" s="184"/>
-      <c r="E42" s="184"/>
-      <c r="F42" s="184"/>
-      <c r="G42" s="184"/>
-      <c r="H42" s="216" t="str">
+      <c r="C42" s="153"/>
+      <c r="D42" s="153"/>
+      <c r="E42" s="153"/>
+      <c r="F42" s="153"/>
+      <c r="G42" s="153"/>
+      <c r="H42" s="182" t="str">
         <f>IF(H37&gt;H41,"Accept H1","Accept H0")</f>
         <v>Accept H0</v>
       </c>
-      <c r="I42" s="184"/>
-      <c r="J42" s="184"/>
-      <c r="K42" s="184"/>
-      <c r="L42" s="184"/>
-      <c r="M42" s="184"/>
-      <c r="N42" s="216" t="str">
+      <c r="I42" s="153"/>
+      <c r="J42" s="153"/>
+      <c r="K42" s="153"/>
+      <c r="L42" s="153"/>
+      <c r="M42" s="153"/>
+      <c r="N42" s="182" t="str">
         <f>IF(N37&gt;N41,"Accept H1","Accept H0")</f>
         <v>Accept H0</v>
       </c>
-      <c r="O42" s="184"/>
-      <c r="P42" s="184"/>
-      <c r="Q42" s="184"/>
-      <c r="R42" s="184"/>
-      <c r="S42" s="184"/>
-      <c r="T42" s="216" t="str">
+      <c r="O42" s="153"/>
+      <c r="P42" s="153"/>
+      <c r="Q42" s="153"/>
+      <c r="R42" s="153"/>
+      <c r="S42" s="153"/>
+      <c r="T42" s="182" t="str">
         <f>IF(T37&gt;T41,"Accept H1","Accept H0")</f>
         <v>Accept H1</v>
       </c>
-      <c r="U42" s="184"/>
-      <c r="V42" s="184"/>
-      <c r="W42" s="184"/>
-      <c r="X42" s="184"/>
-      <c r="Y42" s="185"/>
+      <c r="U42" s="153"/>
+      <c r="V42" s="153"/>
+      <c r="W42" s="153"/>
+      <c r="X42" s="153"/>
+      <c r="Y42" s="154"/>
     </row>
     <row r="43" spans="1:25" ht="19">
-      <c r="A43" s="211" t="s">
+      <c r="A43" s="179" t="s">
         <v>511</v>
       </c>
     </row>
     <row r="45" spans="1:25">
-      <c r="A45" s="211"/>
+      <c r="A45" s="179"/>
     </row>
     <row r="46" spans="1:25">
-      <c r="U46" s="177"/>
-      <c r="V46" s="177"/>
-      <c r="W46" s="217"/>
-      <c r="X46" s="218"/>
-      <c r="Y46" s="217"/>
+      <c r="U46" s="146"/>
+      <c r="V46" s="146"/>
+      <c r="W46" s="183"/>
+      <c r="X46" s="184"/>
+      <c r="Y46" s="183"/>
     </row>
     <row r="47" spans="1:25">
-      <c r="U47" s="177"/>
-      <c r="V47" s="177"/>
-      <c r="W47" s="217"/>
-      <c r="X47" s="218"/>
-      <c r="Y47" s="217"/>
+      <c r="U47" s="146"/>
+      <c r="V47" s="146"/>
+      <c r="W47" s="183"/>
+      <c r="X47" s="184"/>
+      <c r="Y47" s="183"/>
     </row>
     <row r="48" spans="1:25">
-      <c r="U48" s="177"/>
-      <c r="V48" s="177"/>
-      <c r="W48" s="217"/>
-      <c r="X48" s="218"/>
-      <c r="Y48" s="217"/>
+      <c r="U48" s="146"/>
+      <c r="V48" s="146"/>
+      <c r="W48" s="183"/>
+      <c r="X48" s="184"/>
+      <c r="Y48" s="183"/>
     </row>
     <row r="49" spans="21:25">
-      <c r="U49" s="177"/>
-      <c r="V49" s="177"/>
-      <c r="W49" s="217"/>
-      <c r="X49" s="218"/>
-      <c r="Y49" s="217"/>
+      <c r="U49" s="146"/>
+      <c r="V49" s="146"/>
+      <c r="W49" s="183"/>
+      <c r="X49" s="184"/>
+      <c r="Y49" s="183"/>
     </row>
     <row r="50" spans="21:25">
-      <c r="U50" s="177"/>
-      <c r="V50" s="177"/>
-      <c r="W50" s="217"/>
-      <c r="X50" s="218"/>
-      <c r="Y50" s="217"/>
+      <c r="U50" s="146"/>
+      <c r="V50" s="146"/>
+      <c r="W50" s="183"/>
+      <c r="X50" s="184"/>
+      <c r="Y50" s="183"/>
     </row>
     <row r="51" spans="21:25">
-      <c r="U51" s="177"/>
-      <c r="V51" s="177"/>
-      <c r="W51" s="217"/>
-      <c r="X51" s="218"/>
-      <c r="Y51" s="217"/>
+      <c r="U51" s="146"/>
+      <c r="V51" s="146"/>
+      <c r="W51" s="183"/>
+      <c r="X51" s="184"/>
+      <c r="Y51" s="183"/>
     </row>
     <row r="52" spans="21:25">
-      <c r="U52" s="177"/>
-      <c r="V52" s="177"/>
-      <c r="W52" s="217"/>
-      <c r="X52" s="218"/>
-      <c r="Y52" s="217"/>
+      <c r="U52" s="146"/>
+      <c r="V52" s="146"/>
+      <c r="W52" s="183"/>
+      <c r="X52" s="184"/>
+      <c r="Y52" s="183"/>
     </row>
     <row r="53" spans="21:25">
-      <c r="U53" s="177"/>
-      <c r="V53" s="177"/>
-      <c r="W53" s="217"/>
-      <c r="X53" s="218"/>
-      <c r="Y53" s="217"/>
+      <c r="U53" s="146"/>
+      <c r="V53" s="146"/>
+      <c r="W53" s="183"/>
+      <c r="X53" s="184"/>
+      <c r="Y53" s="183"/>
     </row>
     <row r="54" spans="21:25">
-      <c r="U54" s="177"/>
-      <c r="V54" s="177"/>
-      <c r="W54" s="217"/>
-      <c r="X54" s="218"/>
-      <c r="Y54" s="217"/>
+      <c r="U54" s="146"/>
+      <c r="V54" s="146"/>
+      <c r="W54" s="183"/>
+      <c r="X54" s="184"/>
+      <c r="Y54" s="183"/>
     </row>
     <row r="55" spans="21:25">
-      <c r="U55" s="177"/>
-      <c r="V55" s="177"/>
-      <c r="W55" s="217"/>
-      <c r="X55" s="218"/>
-      <c r="Y55" s="217"/>
+      <c r="U55" s="146"/>
+      <c r="V55" s="146"/>
+      <c r="W55" s="183"/>
+      <c r="X55" s="184"/>
+      <c r="Y55" s="183"/>
     </row>
     <row r="56" spans="21:25">
-      <c r="U56" s="177"/>
-      <c r="V56" s="177"/>
-      <c r="W56" s="217"/>
-      <c r="X56" s="218"/>
-      <c r="Y56" s="217"/>
+      <c r="U56" s="146"/>
+      <c r="V56" s="146"/>
+      <c r="W56" s="183"/>
+      <c r="X56" s="184"/>
+      <c r="Y56" s="183"/>
     </row>
     <row r="57" spans="21:25">
-      <c r="U57" s="177"/>
-      <c r="V57" s="177"/>
-      <c r="W57" s="217"/>
-      <c r="X57" s="218"/>
-      <c r="Y57" s="217"/>
+      <c r="U57" s="146"/>
+      <c r="V57" s="146"/>
+      <c r="W57" s="183"/>
+      <c r="X57" s="184"/>
+      <c r="Y57" s="183"/>
     </row>
     <row r="58" spans="21:25">
-      <c r="U58" s="177"/>
-      <c r="V58" s="177"/>
-      <c r="W58" s="217"/>
-      <c r="X58" s="218"/>
-      <c r="Y58" s="217"/>
+      <c r="U58" s="146"/>
+      <c r="V58" s="146"/>
+      <c r="W58" s="183"/>
+      <c r="X58" s="184"/>
+      <c r="Y58" s="183"/>
     </row>
     <row r="59" spans="21:25">
-      <c r="U59" s="177"/>
-      <c r="V59" s="177"/>
-      <c r="W59" s="217"/>
-      <c r="X59" s="218"/>
-      <c r="Y59" s="217"/>
+      <c r="U59" s="146"/>
+      <c r="V59" s="146"/>
+      <c r="W59" s="183"/>
+      <c r="X59" s="184"/>
+      <c r="Y59" s="183"/>
     </row>
     <row r="60" spans="21:25">
-      <c r="U60" s="177"/>
-      <c r="V60" s="177"/>
-      <c r="W60" s="217"/>
-      <c r="X60" s="218"/>
-      <c r="Y60" s="217"/>
+      <c r="U60" s="146"/>
+      <c r="V60" s="146"/>
+      <c r="W60" s="183"/>
+      <c r="X60" s="184"/>
+      <c r="Y60" s="183"/>
     </row>
     <row r="61" spans="21:25">
-      <c r="U61" s="177"/>
-      <c r="V61" s="177"/>
-      <c r="W61" s="217"/>
-      <c r="X61" s="218"/>
-      <c r="Y61" s="217"/>
+      <c r="U61" s="146"/>
+      <c r="V61" s="146"/>
+      <c r="W61" s="183"/>
+      <c r="X61" s="184"/>
+      <c r="Y61" s="183"/>
     </row>
     <row r="62" spans="21:25">
-      <c r="U62" s="177"/>
-      <c r="V62" s="177"/>
-      <c r="W62" s="217"/>
-      <c r="X62" s="218"/>
-      <c r="Y62" s="217"/>
+      <c r="U62" s="146"/>
+      <c r="V62" s="146"/>
+      <c r="W62" s="183"/>
+      <c r="X62" s="184"/>
+      <c r="Y62" s="183"/>
     </row>
     <row r="63" spans="21:25">
-      <c r="U63" s="177"/>
-      <c r="V63" s="177"/>
-      <c r="W63" s="217"/>
-      <c r="X63" s="218"/>
-      <c r="Y63" s="217"/>
+      <c r="U63" s="146"/>
+      <c r="V63" s="146"/>
+      <c r="W63" s="183"/>
+      <c r="X63" s="184"/>
+      <c r="Y63" s="183"/>
     </row>
     <row r="64" spans="21:25">
-      <c r="U64" s="177"/>
-      <c r="V64" s="177"/>
-      <c r="W64" s="217"/>
-      <c r="X64" s="218"/>
-      <c r="Y64" s="217"/>
+      <c r="U64" s="146"/>
+      <c r="V64" s="146"/>
+      <c r="W64" s="183"/>
+      <c r="X64" s="184"/>
+      <c r="Y64" s="183"/>
     </row>
     <row r="65" spans="21:25">
       <c r="U65" s="14"/>
-      <c r="Y65" s="217"/>
+      <c r="Y65" s="183"/>
     </row>
     <row r="66" spans="21:25">
       <c r="U66" s="14"/>
-      <c r="Y66" s="217"/>
+      <c r="Y66" s="183"/>
     </row>
     <row r="67" spans="21:25">
       <c r="U67" s="14"/>
@@ -21316,11 +21246,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="T35:Y35"/>
-    <mergeCell ref="B1:Y1"/>
-    <mergeCell ref="T2:Y2"/>
-    <mergeCell ref="T3:V3"/>
-    <mergeCell ref="W3:Y3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="E3:G3"/>
@@ -21331,6 +21256,11 @@
     <mergeCell ref="K3:M3"/>
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="B2:G2"/>
+    <mergeCell ref="T35:Y35"/>
+    <mergeCell ref="B1:Y1"/>
+    <mergeCell ref="T2:Y2"/>
+    <mergeCell ref="T3:V3"/>
+    <mergeCell ref="W3:Y3"/>
   </mergeCells>
   <phoneticPr fontId="12"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -26127,9 +26057,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
-    <col min="24" max="24" width="3.33203125" style="195" customWidth="1"/>
-    <col min="47" max="47" width="3" style="197" customWidth="1"/>
-    <col min="70" max="70" width="4" style="199" customWidth="1"/>
+    <col min="24" max="24" width="3.33203125" style="164" customWidth="1"/>
+    <col min="47" max="47" width="3" style="166" customWidth="1"/>
+    <col min="70" max="70" width="4" style="168" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:92">
@@ -26178,7 +26108,7 @@
       <c r="T1">
         <v>434</v>
       </c>
-      <c r="X1" s="194"/>
+      <c r="X1" s="163"/>
       <c r="Y1" t="s">
         <v>482</v>
       </c>
@@ -26224,7 +26154,7 @@
       <c r="AQ1">
         <v>434</v>
       </c>
-      <c r="AU1" s="196"/>
+      <c r="AU1" s="165"/>
       <c r="AV1" t="s">
         <v>482</v>
       </c>
@@ -26270,7 +26200,7 @@
       <c r="BN1">
         <v>434</v>
       </c>
-      <c r="BR1" s="198"/>
+      <c r="BR1" s="167"/>
       <c r="BS1" t="s">
         <v>482</v>
       </c>
@@ -31170,7 +31100,7 @@
       <c r="CH32">
         <v>7.2314400000000001E-2</v>
       </c>
-      <c r="CI32" s="190">
+      <c r="CI32" s="159">
         <v>3.0599999999999999E-6</v>
       </c>
       <c r="CJ32">
@@ -32264,7 +32194,7 @@
       </c>
     </row>
     <row r="145" spans="18:18">
-      <c r="R145" s="190"/>
+      <c r="R145" s="159"/>
     </row>
   </sheetData>
   <phoneticPr fontId="12"/>
@@ -32312,115 +32242,115 @@
   <sheetData>
     <row r="1" spans="1:25" s="11" customFormat="1" ht="41" thickBot="1">
       <c r="A1" s="12"/>
-      <c r="B1" s="170" t="s">
+      <c r="B1" s="194" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="171"/>
-      <c r="D1" s="171"/>
-      <c r="E1" s="171"/>
-      <c r="F1" s="171"/>
-      <c r="G1" s="171"/>
-      <c r="H1" s="171"/>
-      <c r="I1" s="171"/>
-      <c r="J1" s="171"/>
-      <c r="K1" s="171"/>
-      <c r="L1" s="171"/>
-      <c r="M1" s="171"/>
-      <c r="N1" s="171"/>
-      <c r="O1" s="171"/>
-      <c r="P1" s="171"/>
-      <c r="Q1" s="171"/>
-      <c r="R1" s="171"/>
-      <c r="S1" s="171"/>
-      <c r="T1" s="171"/>
-      <c r="U1" s="171"/>
-      <c r="V1" s="171"/>
-      <c r="W1" s="171"/>
-      <c r="X1" s="171"/>
-      <c r="Y1" s="171"/>
+      <c r="C1" s="195"/>
+      <c r="D1" s="195"/>
+      <c r="E1" s="195"/>
+      <c r="F1" s="195"/>
+      <c r="G1" s="195"/>
+      <c r="H1" s="195"/>
+      <c r="I1" s="195"/>
+      <c r="J1" s="195"/>
+      <c r="K1" s="195"/>
+      <c r="L1" s="195"/>
+      <c r="M1" s="195"/>
+      <c r="N1" s="195"/>
+      <c r="O1" s="195"/>
+      <c r="P1" s="195"/>
+      <c r="Q1" s="195"/>
+      <c r="R1" s="195"/>
+      <c r="S1" s="195"/>
+      <c r="T1" s="195"/>
+      <c r="U1" s="195"/>
+      <c r="V1" s="195"/>
+      <c r="W1" s="195"/>
+      <c r="X1" s="195"/>
+      <c r="Y1" s="195"/>
     </row>
     <row r="2" spans="1:25" ht="19" thickBot="1">
-      <c r="A2" s="152" t="s">
+      <c r="A2" s="201" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="168" t="s">
+      <c r="B2" s="217" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="169"/>
-      <c r="D2" s="169"/>
-      <c r="E2" s="169"/>
-      <c r="F2" s="169"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="166" t="s">
+      <c r="C2" s="218"/>
+      <c r="D2" s="218"/>
+      <c r="E2" s="218"/>
+      <c r="F2" s="218"/>
+      <c r="G2" s="218"/>
+      <c r="H2" s="212" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="167"/>
-      <c r="J2" s="167"/>
-      <c r="K2" s="167"/>
-      <c r="L2" s="167"/>
-      <c r="M2" s="167"/>
-      <c r="N2" s="158" t="s">
+      <c r="I2" s="213"/>
+      <c r="J2" s="213"/>
+      <c r="K2" s="213"/>
+      <c r="L2" s="213"/>
+      <c r="M2" s="213"/>
+      <c r="N2" s="207" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="159"/>
-      <c r="P2" s="159"/>
-      <c r="Q2" s="159"/>
-      <c r="R2" s="159"/>
-      <c r="S2" s="159"/>
-      <c r="T2" s="172" t="s">
+      <c r="O2" s="208"/>
+      <c r="P2" s="208"/>
+      <c r="Q2" s="208"/>
+      <c r="R2" s="208"/>
+      <c r="S2" s="208"/>
+      <c r="T2" s="196" t="s">
         <v>50</v>
       </c>
-      <c r="U2" s="173"/>
-      <c r="V2" s="173"/>
-      <c r="W2" s="173"/>
-      <c r="X2" s="173"/>
-      <c r="Y2" s="173"/>
+      <c r="U2" s="197"/>
+      <c r="V2" s="197"/>
+      <c r="W2" s="197"/>
+      <c r="X2" s="197"/>
+      <c r="Y2" s="197"/>
     </row>
     <row r="3" spans="1:25" ht="19" thickBot="1">
-      <c r="A3" s="153"/>
-      <c r="B3" s="155" t="s">
+      <c r="A3" s="202"/>
+      <c r="B3" s="204" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="156"/>
-      <c r="D3" s="156"/>
-      <c r="E3" s="155" t="s">
+      <c r="C3" s="205"/>
+      <c r="D3" s="205"/>
+      <c r="E3" s="204" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="156"/>
-      <c r="G3" s="157"/>
-      <c r="H3" s="165" t="s">
+      <c r="F3" s="205"/>
+      <c r="G3" s="206"/>
+      <c r="H3" s="215" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="163"/>
-      <c r="J3" s="164"/>
-      <c r="K3" s="163" t="s">
+      <c r="I3" s="214"/>
+      <c r="J3" s="216"/>
+      <c r="K3" s="214" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="163"/>
-      <c r="M3" s="163"/>
-      <c r="N3" s="160" t="s">
+      <c r="L3" s="214"/>
+      <c r="M3" s="214"/>
+      <c r="N3" s="209" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="161"/>
-      <c r="P3" s="161"/>
-      <c r="Q3" s="160" t="s">
+      <c r="O3" s="210"/>
+      <c r="P3" s="210"/>
+      <c r="Q3" s="209" t="s">
         <v>34</v>
       </c>
-      <c r="R3" s="161"/>
-      <c r="S3" s="162"/>
-      <c r="T3" s="174" t="s">
+      <c r="R3" s="210"/>
+      <c r="S3" s="211"/>
+      <c r="T3" s="198" t="s">
         <v>24</v>
       </c>
-      <c r="U3" s="175"/>
-      <c r="V3" s="175"/>
-      <c r="W3" s="174" t="s">
+      <c r="U3" s="199"/>
+      <c r="V3" s="199"/>
+      <c r="W3" s="198" t="s">
         <v>34</v>
       </c>
-      <c r="X3" s="175"/>
-      <c r="Y3" s="176"/>
+      <c r="X3" s="199"/>
+      <c r="Y3" s="200"/>
     </row>
     <row r="4" spans="1:25" ht="20" thickBot="1">
-      <c r="A4" s="154"/>
+      <c r="A4" s="203"/>
       <c r="B4" s="67" t="s">
         <v>20</v>
       </c>
@@ -32813,7 +32743,7 @@
       </c>
     </row>
     <row r="11" spans="1:25" ht="20" thickBot="1">
-      <c r="A11" s="180" t="s">
+      <c r="A11" s="149" t="s">
         <v>478</v>
       </c>
       <c r="B11" s="37"/>
@@ -32972,7 +32902,7 @@
       </c>
     </row>
     <row r="14" spans="1:25" ht="20" thickBot="1">
-      <c r="A14" s="180" t="s">
+      <c r="A14" s="149" t="s">
         <v>470</v>
       </c>
       <c r="B14" s="37"/>
@@ -33449,7 +33379,7 @@
       </c>
     </row>
     <row r="23" spans="1:25" ht="20" thickBot="1">
-      <c r="A23" s="180" t="s">
+      <c r="A23" s="149" t="s">
         <v>467</v>
       </c>
       <c r="B23" s="37"/>
@@ -33824,11 +33754,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="T3:V3"/>
-    <mergeCell ref="W3:Y3"/>
-    <mergeCell ref="B1:Y1"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="H2:M2"/>
@@ -33838,6 +33763,11 @@
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="K3:M3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="T3:V3"/>
+    <mergeCell ref="W3:Y3"/>
+    <mergeCell ref="B1:Y1"/>
   </mergeCells>
   <phoneticPr fontId="12"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>